<commit_message>
Added Commonness, Avoid, Feral, and added plants
* Added more plants to the library
		* Added Commonness, Avoid, Feral
</commit_message>
<xml_diff>
--- a/Assets/Data/Plants.xlsx
+++ b/Assets/Data/Plants.xlsx
@@ -8,33 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity Projects\GitHub\Edible Plants\Assets\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E33A44-A1F1-4444-9697-BE318BA10D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E84B3D2-7732-4536-B60B-6D8DD5B95BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32685" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{C257811F-7D87-40D1-8DDB-E1E2C9270973}"/>
+    <workbookView xWindow="28860" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plants" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Latin Name</t>
   </si>
@@ -45,20 +31,670 @@
     <t>Info</t>
   </si>
   <si>
+    <t>Root</t>
+  </si>
+  <si>
+    <t>Stem</t>
+  </si>
+  <si>
+    <t>Leafs</t>
+  </si>
+  <si>
+    <t>Flower</t>
+  </si>
+  <si>
+    <t>Seeds</t>
+  </si>
+  <si>
     <t>Angelica archangelica</t>
   </si>
   <si>
     <t>Kvanne</t>
+  </si>
+  <si>
+    <t>Kvanne (Angelica archangelica) är en tvåårig ört tillhörande familjen flockblommiga växter. Plantan har ofta en stark lukt, i synnerhet underarten strandkvanne. Båda underarterna har grova rötter och upprepat sammansatta blad där småbladen är grovt sågade. Stjälken är ihålig, slät och kan ofta ha en rödaktig ton. Under plantans första år har den inga blommor utan endast blad som växer mer eller mindre direkt ifrån marken. Det är först under plantans andra år som den når sin fulla höjd och de blekgröna blommorna slår ut.</t>
+  </si>
+  <si>
+    <t>Urtica dioica</t>
+  </si>
+  <si>
+    <t>Brännässla</t>
+  </si>
+  <si>
+    <t>Brännässla (Urtica dioica) är en art i familjen nässelväxter. Arten är allmän över hela Nordeuropa, men förekommer även i övriga Europa, Asien, Nordafrika och Nordamerika.</t>
+  </si>
+  <si>
+    <t>Lamium album</t>
+  </si>
+  <si>
+    <t>Vitplister</t>
+  </si>
+  <si>
+    <t>Vitplister är mångårig med jordstam. Den har lång blomningstid (maj-september). Arten växer gärna på odlad mark, i täta bestånd vid vägar, gator och murar. Den är vanlig i Sveriges östra  Örtståndet producerar en eterisk olja med mycket frän lukt. De späda skotten som kommer tidigt på våren har trots det förr använts som grönkål. De tidigaste skotten av vitplister är lätta att förväxla med nässelskott, då dessa samlas för att användas som kål, och de två växer ofta tillsammans.</t>
+  </si>
+  <si>
+    <t>Lamium purpureum</t>
+  </si>
+  <si>
+    <t>Rödplister</t>
+  </si>
+  <si>
+    <t>Rödplister (Lamium purpureum) är en ettårig, cirka 30 centimeter hög ört med purpurröda blommor. Unga blad är också purpurfärgade, men blir gröna med tiden. Den röda färgen dröjer kvar längst i spetsarna av bladen. Rödplister förekommer över större delen av Europa och i Asien. Den förekommer även tidvis, som ogräs vid odlad mark, i Nordamerika.</t>
+  </si>
+  <si>
+    <t>Achillea millefolium</t>
+  </si>
+  <si>
+    <t>Röllika</t>
+  </si>
+  <si>
+    <t>Röllika blommar hela sommaren och långt in på hösten, men ger ingen nektar. Pollineras ändå av insekter, som besöker blomman för frömjölets skull.</t>
+  </si>
+  <si>
+    <t>Chamaenerion angustifolium</t>
+  </si>
+  <si>
+    <t>Mjölke</t>
+  </si>
+  <si>
+    <t>Mjölke finns i norra halvklotets tempererade områden. Den är vanlig längs banvallar, på hyggen och diken i hela Sverige, ända upp på kalfjället. På 1950-talet nådde den enligt en inventering i Jämtland 1 120 m, 2008 har den klättrat upp till 1 380 m. Oberoende undersökningar i Uralbergen, Alperna, Pyrenéerna och Jurabergen har visat liknande tendenser. Orsaken antas vara den globala uppvärmningen</t>
+  </si>
+  <si>
+    <t>Typha</t>
+  </si>
+  <si>
+    <t>Kaveldun</t>
+  </si>
+  <si>
+    <t>Kaveldunsläktet (Typha)[1][2] är ett släkte i familjen kaveldunsväxter[1]. Släktet har 8–15 arter som förekommer i nästan hela världen. Släktet beskrevs först av Carl von Linné. I Sverige finns arterna bredkaveldun (T. latifolia) och smalkaveldun (T. angustifolia)</t>
+  </si>
+  <si>
+    <t>Svinmålla</t>
+  </si>
+  <si>
+    <t>Chenopodium album</t>
+  </si>
+  <si>
+    <r>
+      <t>Svinmålla</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Chenopodium album</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) är en ört. Den förekommer ofta, som "ogräs", i trädgårdsland och andra marker med bar jord. Bladen kan användas på samma sätt som spenat. Svinmålla är vanlig i norra Indien som gröda för mat.</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">1] I engelska texter kallas den ibland vid sitt hindi-namn </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bathua</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> eller </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bathuwa.</t>
+    </r>
+  </si>
+  <si>
+    <t>Vanlighet</t>
+  </si>
+  <si>
+    <t>Våtarv (Stellaria media) är ett mycket vanligt och rikligt förekommande ogräs i världen. I Sverige är våtarv det vanligaste örtogräset.</t>
+  </si>
+  <si>
+    <t>Stellaria media</t>
+  </si>
+  <si>
+    <t>Våtarv</t>
+  </si>
+  <si>
+    <t>Åkerspergel</t>
+  </si>
+  <si>
+    <t>Åkerspärgel (Spergula arvensis L.) är en ettårig lågväxande ört. Ursprungligen stavades svenska namnet åkerspergel.</t>
+  </si>
+  <si>
+    <t>Spergula arvensis</t>
+  </si>
+  <si>
+    <r>
+      <t>Körsbärskornell</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cornus mas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) är en växtart i familjen kornellväxter och förekommer naturligt från centrala och sydöstra Europa till Kaukasus. I Sverige förekommer den inte naturligt, utan som prydnadsväxt eller som bärbuske i trädgårdar och parker. Körsbärskornell är en lövfällande buske (4 meter hög) eller ett litet träd (8 meter), med bred och ganska låg krona. Buskformen har fler upprättstående huvudgrenar, medan trädformen har en genomgående stam och överhängande huvudgrenar som går ganska vågrätt ut från huvudstammen. Barken är först gråbrun med gröna inslag. Senare blir den ljusbrun med spridda korkporer och till sist är den grå och uppsprickande. Knopparna är motsatt placerade på grenen, bruna och spetsiga (blomknopparna är dock runda och utspärrade). Avståndet mellan knopparna är långt. Bladen är äggrunda, med lång spets. Bladkanten är helbreddad och bladets ådror är bågformade. Översidan är skinande grön, medan undersidan är blågrön. Höstfärgen är brungul.</t>
+    </r>
+  </si>
+  <si>
+    <t>Körsbärskornell</t>
+  </si>
+  <si>
+    <t>Cornus mas</t>
+  </si>
+  <si>
+    <t>Berries</t>
+  </si>
+  <si>
+    <t>Hönsbär</t>
+  </si>
+  <si>
+    <t>Hönsbär är en 10-25 cm hög och flerårig ört.[1] I flera avseenden liknar den skogskornell (C. sanguinea), men i andra avseenden skiljer den sig, särskilt när det gäller blomningen. Den har nämligen mycket små blommor som till alla sina delar utom ståndarna är svartröda.[1] För att insekter ändå ska lockas (jämför avsnitt Etymologi nedan), har växten en "sammansatt blomma" med ett stort och lysande skenbart blomhylle, genom att de fyra översta bladen omvandlats till högblad av vit färg som sitter i en krans som ett svepe, men härmande en blomkrona. I mitten är den lilla svartvioletta blomställningen samlad, en enkel flock.</t>
+  </si>
+  <si>
+    <t>Cornus suecica</t>
+  </si>
+  <si>
+    <t>Björnlokan</t>
+  </si>
+  <si>
+    <t>Heracleum sphondylium</t>
+  </si>
+  <si>
+    <t>Avoid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Björnlokan är en stor, grov och flerårig ört, som tämligen allmänt förekommer på ängar och vägkanter genom större delen av Sveriges floraområde, ungefär upp till polcirkeln. Den blommar under högsommaren. Björnlokan kan orsaka stor sveda om den kommer i kontakt med huden hos människor[3]. Björnloka och jätteloka innehåller furanokumariner som är irriterande på hud, särskilt om huden utsätts för solbestrålning (fotosensibilisering).[4] Brännskadeliknande symtom med kraftig hudirritation, rodnad och blåsor, som kan bli stora och smärtsamma. Besvären kan kvarstå i veckor, eventuellt även ärrbildning och mörkfärgning av huden. </t>
+  </si>
+  <si>
+    <t>Vildmorot</t>
+  </si>
+  <si>
+    <r>
+      <t>Vildmorot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Daucus carota</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) är en art i familjen flockblommiga växter. I likhet med alla övriga arter i morotssläktet är växten tvåårig. Den förädlade moroten (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>D. carota sativa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) klassas som en underart. Den förekommer i Eurasien och Nordafrika. Människan har spridit den till Amerika, där den blivit ett svårt ogräs. Till skillnad från den förädlade moroten har vildmoroten en tunn, träig pålrot - som dock ändå är ätlig.</t>
+    </r>
+  </si>
+  <si>
+    <t>Daucus carota</t>
+  </si>
+  <si>
+    <t>Palsternacka</t>
+  </si>
+  <si>
+    <t>Palsternacka odlades redan i antikens Grekland. I Sverige omtalas den på 1500-talet, men tycks ha odlats långt tidigare, och var under medeltiden och renässansen betydligt mer populär som grönsak än idag. Den förekommer ofta i väg och dikeskanter och uppträder även som ogräs. Enligt SVA "Vildpalsternacka orsakar ökad känslighet för solljus (fotosensibilisering) och hudskador, men kan även orsaka förändringar i ögonen".</t>
+  </si>
+  <si>
+    <t>Pastinaca sativa</t>
+  </si>
+  <si>
+    <r>
+      <t>Kärrsiljan är omkring en meter hög och förekommer allmänt på kärrängar och stränder i så gott som hela Sverige och Finland.</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1]</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2] I Norge förekommer den endast söder om fjällen.</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2] I övrigt är den inhemsk i nästan hela Europa.</t>
+    </r>
+  </si>
+  <si>
+    <t>Kärrsilja</t>
+  </si>
+  <si>
+    <t>Peucedanum palustre</t>
+  </si>
+  <si>
+    <r>
+      <t>Strätta</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Angelica sylvestris)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> är en flerårig ört i släktet kvannar (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Angelica</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) och familjen flockblommiga växter. Strättan är en mycket storvuxen ört med flikiga blad och stora vita eller rosa blomflockar, och förekommer i hela Europa och stora delar av Asien. Den återfinns framför allt på fuktig mark, bland annat på stränder och ängar samt på mänskligt störd mark som vägrenar och betesmarker. Roten har en aromatisk doft, och strättan har tidigare använts som färgväxt, i medicinen samt till örtte och mjöl.</t>
+    </r>
+  </si>
+  <si>
+    <t>Strätta</t>
+  </si>
+  <si>
+    <t>Angelica sylvestris</t>
+  </si>
+  <si>
+    <t>Fänkål blir cirka 1,5 meter hög. Bladen är mycket finflikiga (dilliknande) och doftar aromatiskt och lakritsliknande. Hela växten innehåller eteriska oljor. Under blomningstiden utvecklas ganska bleka stjälkar, med kraftiga förtjockningar vid markytan.</t>
+  </si>
+  <si>
+    <t>Fänkål</t>
+  </si>
+  <si>
+    <t>Foeniculum vulgare</t>
+  </si>
+  <si>
+    <t>Förvildad</t>
+  </si>
+  <si>
+    <r>
+      <t>Libbsticka,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Levisticum officinale</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> W.D.J.Koch, även kallad </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>selleriört</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, är en flerårig växt inom familjen flockblommiga växter. Växten används som krydda och fördes på medeltiden till Sverige av munkar.</t>
+    </r>
+  </si>
+  <si>
+    <t>Libbsticka</t>
+  </si>
+  <si>
+    <t>Levisticum officinale</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -72,6 +708,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,16 +722,197 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -96,17 +920,206 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -417,21 +1430,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4D11510-A1CD-4592-931A-B69E92B4EF4A}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="4" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -441,17 +1454,422 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="K14">
         <v>4</v>
       </c>
     </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="K16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C10" r:id="rId1" tooltip="Ogräs" display="https://sv.wikipedia.org/wiki/Ogr%C3%A4s" xr:uid="{20AF4F85-92C6-47E9-B9BE-D7E0DA55EC47}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Plants now got 30
* Added Plants now got 30
</commit_message>
<xml_diff>
--- a/Assets/Data/Plants.xlsx
+++ b/Assets/Data/Plants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity Projects\GitHub\Edible Plants\Assets\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E84B3D2-7732-4536-B60B-6D8DD5B95BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A12D57C-97E6-4E5C-A481-5EDB1BA5648F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28860" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
   <si>
     <t>Latin Name</t>
   </si>
@@ -115,95 +115,6 @@
     <t>Chenopodium album</t>
   </si>
   <si>
-    <r>
-      <t>Svinmålla</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Chenopodium album</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) är en ört. Den förekommer ofta, som "ogräs", i trädgårdsland och andra marker med bar jord. Bladen kan användas på samma sätt som spenat. Svinmålla är vanlig i norra Indien som gröda för mat.</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">1] I engelska texter kallas den ibland vid sitt hindi-namn </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>bathua</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> eller </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>bathuwa.</t>
-    </r>
-  </si>
-  <si>
     <t>Vanlighet</t>
   </si>
   <si>
@@ -216,51 +127,12 @@
     <t>Våtarv</t>
   </si>
   <si>
-    <t>Åkerspergel</t>
-  </si>
-  <si>
     <t>Åkerspärgel (Spergula arvensis L.) är en ettårig lågväxande ört. Ursprungligen stavades svenska namnet åkerspergel.</t>
   </si>
   <si>
     <t>Spergula arvensis</t>
   </si>
   <si>
-    <r>
-      <t>Körsbärskornell</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cornus mas</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) är en växtart i familjen kornellväxter och förekommer naturligt från centrala och sydöstra Europa till Kaukasus. I Sverige förekommer den inte naturligt, utan som prydnadsväxt eller som bärbuske i trädgårdar och parker. Körsbärskornell är en lövfällande buske (4 meter hög) eller ett litet träd (8 meter), med bred och ganska låg krona. Buskformen har fler upprättstående huvudgrenar, medan trädformen har en genomgående stam och överhängande huvudgrenar som går ganska vågrätt ut från huvudstammen. Barken är först gråbrun med gröna inslag. Senare blir den ljusbrun med spridda korkporer och till sist är den grå och uppsprickande. Knopparna är motsatt placerade på grenen, bruna och spetsiga (blomknopparna är dock runda och utspärrade). Avståndet mellan knopparna är långt. Bladen är äggrunda, med lång spets. Bladkanten är helbreddad och bladets ådror är bågformade. Översidan är skinande grön, medan undersidan är blågrön. Höstfärgen är brungul.</t>
-    </r>
-  </si>
-  <si>
     <t>Körsbärskornell</t>
   </si>
   <si>
@@ -273,9 +145,6 @@
     <t>Hönsbär</t>
   </si>
   <si>
-    <t>Hönsbär är en 10-25 cm hög och flerårig ört.[1] I flera avseenden liknar den skogskornell (C. sanguinea), men i andra avseenden skiljer den sig, särskilt när det gäller blomningen. Den har nämligen mycket små blommor som till alla sina delar utom ståndarna är svartröda.[1] För att insekter ändå ska lockas (jämför avsnitt Etymologi nedan), har växten en "sammansatt blomma" med ett stort och lysande skenbart blomhylle, genom att de fyra översta bladen omvandlats till högblad av vit färg som sitter i en krans som ett svepe, men härmande en blomkrona. I mitten är den lilla svartvioletta blomställningen samlad, en enkel flock.</t>
-  </si>
-  <si>
     <t>Cornus suecica</t>
   </si>
   <si>
@@ -288,212 +157,24 @@
     <t>Avoid</t>
   </si>
   <si>
-    <t xml:space="preserve">Björnlokan är en stor, grov och flerårig ört, som tämligen allmänt förekommer på ängar och vägkanter genom större delen av Sveriges floraområde, ungefär upp till polcirkeln. Den blommar under högsommaren. Björnlokan kan orsaka stor sveda om den kommer i kontakt med huden hos människor[3]. Björnloka och jätteloka innehåller furanokumariner som är irriterande på hud, särskilt om huden utsätts för solbestrålning (fotosensibilisering).[4] Brännskadeliknande symtom med kraftig hudirritation, rodnad och blåsor, som kan bli stora och smärtsamma. Besvären kan kvarstå i veckor, eventuellt även ärrbildning och mörkfärgning av huden. </t>
-  </si>
-  <si>
     <t>Vildmorot</t>
   </si>
   <si>
-    <r>
-      <t>Vildmorot</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Daucus carota</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) är en art i familjen flockblommiga växter. I likhet med alla övriga arter i morotssläktet är växten tvåårig. Den förädlade moroten (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D. carota sativa</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) klassas som en underart. Den förekommer i Eurasien och Nordafrika. Människan har spridit den till Amerika, där den blivit ett svårt ogräs. Till skillnad från den förädlade moroten har vildmoroten en tunn, träig pålrot - som dock ändå är ätlig.</t>
-    </r>
-  </si>
-  <si>
     <t>Daucus carota</t>
   </si>
   <si>
     <t>Palsternacka</t>
   </si>
   <si>
-    <t>Palsternacka odlades redan i antikens Grekland. I Sverige omtalas den på 1500-talet, men tycks ha odlats långt tidigare, och var under medeltiden och renässansen betydligt mer populär som grönsak än idag. Den förekommer ofta i väg och dikeskanter och uppträder även som ogräs. Enligt SVA "Vildpalsternacka orsakar ökad känslighet för solljus (fotosensibilisering) och hudskador, men kan även orsaka förändringar i ögonen".</t>
-  </si>
-  <si>
     <t>Pastinaca sativa</t>
   </si>
   <si>
-    <r>
-      <t>Kärrsiljan är omkring en meter hög och förekommer allmänt på kärrängar och stränder i så gott som hela Sverige och Finland.</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1]</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2] I Norge förekommer den endast söder om fjällen.</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2] I övrigt är den inhemsk i nästan hela Europa.</t>
-    </r>
-  </si>
-  <si>
     <t>Kärrsilja</t>
   </si>
   <si>
     <t>Peucedanum palustre</t>
   </si>
   <si>
-    <r>
-      <t>Strätta</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Angelica sylvestris)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> är en flerårig ört i släktet kvannar (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Angelica</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) och familjen flockblommiga växter. Strättan är en mycket storvuxen ört med flikiga blad och stora vita eller rosa blomflockar, och förekommer i hela Europa och stora delar av Asien. Den återfinns framför allt på fuktig mark, bland annat på stränder och ängar samt på mänskligt störd mark som vägrenar och betesmarker. Roten har en aromatisk doft, och strättan har tidigare använts som färgväxt, i medicinen samt till örtte och mjöl.</t>
-    </r>
-  </si>
-  <si>
     <t>Strätta</t>
   </si>
   <si>
@@ -510,6 +191,120 @@
   </si>
   <si>
     <t>Förvildad</t>
+  </si>
+  <si>
+    <t>Libbsticka</t>
+  </si>
+  <si>
+    <t>Levisticum officinale</t>
+  </si>
+  <si>
+    <t>Palsternacka odlades redan i antikens Grekland. I Sverige omtalas den på 1500-talet, men tycks ha odlats långt tidigare, och var under medeltiden och renässansen betydligt mer populär som grönsak än idag. Den förekommer ofta i väg och dikeskanter och uppträder även som ogräs. Enligt SVA Vildpalsternacka orsakar ökad känslighet för solljus (fotosensibilisering) och hudskador, men kan även orsaka förändringar i ögonen.</t>
+  </si>
+  <si>
+    <t>Björnlokan är en stor, grov och flerårig ört, som tämligen allmänt förekommer på ängar och vägkanter genom större delen av Sveriges floraområde, ungefär upp till polcirkeln. Den blommar under högsommaren. Björnlokan kan orsaka stor sveda om den kommer i kontakt med huden hos människor. Björnloka och jätteloka innehåller furanokumariner som är irriterande på hud, särskilt om huden utsätts för solbestrålning (fotosensibilisering).</t>
+  </si>
+  <si>
+    <t>Kärrsiljan är omkring en meter hög och förekommer allmänt på kärrängar och stränder i så gott som hela Sverige och Finland. I Norge förekommer den endast söder om fjällen. I övrigt är den inhemsk i nästan hela Europa.</t>
+  </si>
+  <si>
+    <t>Hönsbär är en 10-25 cm hög och flerårig ört. I flera avseenden liknar den skogskornell (C. sanguinea), men i andra avseenden skiljer den sig, särskilt när det gäller blomningen. Den har nämligen mycket små blommor som till alla sina delar utom ståndarna är svartröda.</t>
+  </si>
+  <si>
+    <t>Åkerspärgel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kirskål kan bli upp till 80 cm hög. De bredbladiga bladen är två gånger 3-fingrade med tandad kant. De små vita blommorna sitter samlade i flockar, och pollineras framförallt av flugor och skalbaggar. I Sverige är kirskålen begränsad till den sydliga hälften av floraområdet. Är där vanlig i parker och gamla trädgårdar, men mindre vanlig i lundskogar och på inägor. </t>
+  </si>
+  <si>
+    <t>Kirskål</t>
+  </si>
+  <si>
+    <t>Aegopodium podagraria</t>
+  </si>
+  <si>
+    <t>Bockrot</t>
+  </si>
+  <si>
+    <t>Pimpinella saxifraga</t>
+  </si>
+  <si>
+    <t>Carum carvi</t>
+  </si>
+  <si>
+    <t>Kummin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kummin har en mycket lång historia och kan spåras tillbaka till sumererna, som kallade kryddan gamun. De torkade frukterna (ofta felaktigt benämnda frön) används som krydda till exempelvis bröd, korv, ost och soppor. De används också för smaksättning av kryddat brännvin (akvavit). </t>
+  </si>
+  <si>
+    <t>Mycket lätt att förväxla med Vildpersilja som är mycket giftig. Undvik. Persilja är en tvåårig växt som blommar det andra året. Första året blir det bara en liten marknära bladrosett. Persilja är mycket rik på karoten (som omvandlas till A-vitamin i kroppen), B-vitaminer och C-vitamin samt järn och kalcium. Den är robust och tålig. Kan bli upp till 70 cm hög. Bladen är upprepat parflikiga. Det förekommer även framodlade sorter med starkt krusiga blad, "kruspersilja".</t>
+  </si>
+  <si>
+    <t>Persilja</t>
+  </si>
+  <si>
+    <t>Petroselinum crispum</t>
+  </si>
+  <si>
+    <t>Aethusa cynapium</t>
+  </si>
+  <si>
+    <t>Vildpersilja</t>
+  </si>
+  <si>
+    <t>Hela växten är mycket giftig, särskilt fröna. Förtäring medför kraftigt illamående, kräkning, diarré, stark salivavsöndring, muskelryckningar, smärta i buken och muskler, svårighet att röra på armarna och benen, sluddrande tal, dvala.[1] Många av följderna liknar dem hos epilepsi. Förgiftningar behandlas med magpumpning och därefter dryck.</t>
+  </si>
+  <si>
+    <t>Selleri</t>
+  </si>
+  <si>
+    <t>Apium graveolens</t>
+  </si>
+  <si>
+    <t>Coriandrum sativum</t>
+  </si>
+  <si>
+    <t>Koriander</t>
+  </si>
+  <si>
+    <t>Finns vildväxande enbart i Europa, huvudsakligen i lägre områden omslutande Alpernas västra del och på liknande vis runt Pyrenéerna. I Sverige ursprungligen enbart som odlad kryddväxt, men kan finnas förvildad i närheten av kulturpåverkade områden.</t>
+  </si>
+  <si>
+    <t>Spansk körvel</t>
+  </si>
+  <si>
+    <t>Myrrhis odorata</t>
+  </si>
+  <si>
+    <t>Arten är ursprunglig i östra Europa och västra Asien, från Schweiz och Polen till norra Iran, men har introducerats i större delen av övriga Europa och på flera platser i Nordamerika och Nordafrika. I Sverige är den inte ursprunglig, men är bofast och reproducerande i södra delen av landet, till Uppland och Dalarna. Bladen används färska, torkade eller frysta som krydda till bland annat soppa, sås, sallad, kyckling, ägg- och fiskrätter. Som krydda ingår den i kryddblandningen fines herbes. Smaken påminner om anis.</t>
+  </si>
+  <si>
+    <t>Dansk körvel</t>
+  </si>
+  <si>
+    <t>Anthriscus cerefolium</t>
+  </si>
+  <si>
+    <t>Hundkäx (Anthriscus sylvestris) (L.) Hoffm. är en allmänt förekommande växt som tillhör släktet småkörvlar (Anthriscus). I Sverige förekommer hundkäx allmänt i hela landet och utgör den mest förekommande arten ur familjen flockblommiga växter. Stundtals går den till och med att återfinna ovanför trädgränsen, dock enbart tillfälligt. Hundkäx kan framförallt sammanblandas med spansk körvel (Myrrhis odorata), odört (Conium maculatum) samt vildpersilja (Aethusa cynapium).</t>
+  </si>
+  <si>
+    <t>Hundkäx</t>
+  </si>
+  <si>
+    <t>Anthriscus sylvestris</t>
+  </si>
+  <si>
+    <t>Svinmålla (Chenopodium album) är en ört. Den förekommer ofta, som "ogräs", i trädgårdsland och andra marker med bar jord. Bladen kan användas på samma sätt som spenat. Svinmålla är vanlig i norra Indien som gröda för mat.[1] I engelska texter kallas den ibland vid sitt hindi-namn bathua eller bathuwa.</t>
+  </si>
+  <si>
+    <t>Körsbärskornell (Cornus mas) är en växtart i familjen kornellväxter och förekommer naturligt från centrala och sydöstra Europa till Kaukasus. Körsbärskornell är en lövfällande buske (4 meter hög) eller ett litet träd (8 meter), med bred och ganska låg krona. Bladen är äggrunda, med lång spets.</t>
+  </si>
+  <si>
+    <t>Vildmorot (Daucus carota) är en art i familjen flockblommiga växter. I likhet med alla övriga arter i morotssläktet är växten tvåårig. Den förädlade moroten (D. carota sativa) klassas som en underart. Den förekommer i Eurasien och Nordafrika. Människan har spridit den till Amerika, där den blivit ett svårt ogräs. Till skillnad från den förädlade moroten har vildmoroten en tunn, träig pålrot - som dock ändå är ätlig.</t>
+  </si>
+  <si>
+    <t>Strätta (Angelica sylvestris) är en flerårig ört i släktet kvannar (Angelica) och familjen flockblommiga växter. Strättan är en mycket storvuxen ört med flikiga blad och stora vita eller rosa blomflockar, och förekommer i hela Europa och stora delar av Asien. Den återfinns framför allt på fuktig mark, bland annat på stränder och ängar samt på mänskligt störd mark som vägrenar och betesmarker. Roten har en aromatisk doft, och strättan har tidigare använts som färgväxt, i medicinen samt till örtte och mjöl.</t>
   </si>
   <si>
     <r>
@@ -548,7 +343,6 @@
     </r>
     <r>
       <rPr>
-        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -569,17 +363,20 @@
     </r>
   </si>
   <si>
-    <t>Libbsticka</t>
-  </si>
-  <si>
-    <t>Levisticum officinale</t>
+    <t>Bockrot, vanlig bockrot eller backanis (Pimpinella saxifraga) är flerårig med en så kallad "månghövdad pålrot", det vill säga en kort kandelaberstam, uppburen av pålroten. Den växer allmänt på torra ängsbackar genom nästan hela Skandinavien. Roten är seg, smal och mycket djupgående, den har en brännande aromatisk smak och brukades förr som ett magstärkande och slemlösande läkemedel, till te mot hosta med mera. Den fanns med i den svenska farmakopén från 1775 fram till 1908 och såldes även på apoteken under de båda världskrigen. Ett extrakt av roten ingick bland annat i "Pimpinelladroppar" mot heshet och halsont</t>
+  </si>
+  <si>
+    <t>Selleri (Apium graveolens) är en tvåårig, starkt doftande ört, som växer vilt i Europa, västra Asien och Nordafrika. Selleri har en lång historia som krydd- och medicinalväxt och den äts även som grönsak och rotfrukt. Det är främst roten, stjälken och fröna som används men även blad kan användas.</t>
+  </si>
+  <si>
+    <t>Koriander har sitt ursprung i Sydeuropa och Asien. De torkade fröna har en kryddig, nötaktig behaglig smak. Bladen har en svårdefinierad aromatisk lukt och smak, som inte alla tycker om. Bladen används i asiatisk matlagning ungefär som man i Sverige använder persilja.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -716,14 +513,6 @@
     </font>
     <font>
       <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1072,9 +861,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -1431,55 +1219,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="4" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>65</v>
+      <c r="J1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1625,17 +1414,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="2">
+      <c r="C9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9">
         <v>1</v>
       </c>
       <c r="E9">
@@ -1650,13 +1439,13 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" t="s">
-        <v>35</v>
-      </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -1673,13 +1462,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -1696,13 +1485,13 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>92</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -1715,14 +1504,14 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>45</v>
+      <c r="A13" t="s">
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -1732,14 +1521,14 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>47</v>
+      <c r="A14" t="s">
+        <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -1750,13 +1539,13 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
+        <v>93</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -1766,14 +1555,14 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>55</v>
+      <c r="A16" t="s">
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D16">
         <v>3</v>
@@ -1782,15 +1571,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>58</v>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1801,13 +1590,13 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>94</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -1820,14 +1609,14 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>64</v>
+      <c r="A19" t="s">
+        <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -1850,19 +1639,252 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
+      </c>
+      <c r="C20" t="s">
+        <v>95</v>
       </c>
       <c r="D20">
         <v>3</v>
       </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
       <c r="L20">
         <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Border, better visuals, text fixes
* Made a border around the game, added backgrounds to text answers
		* Corrected text
</commit_message>
<xml_diff>
--- a/Assets/Data/Plants.xlsx
+++ b/Assets/Data/Plants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity Projects\GitHub\Edible Plants\Assets\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A12D57C-97E6-4E5C-A481-5EDB1BA5648F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C5B371A-6878-429C-8978-DAC89C0B3093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28860" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,9 +106,6 @@
     <t>Kaveldun</t>
   </si>
   <si>
-    <t>Kaveldunsläktet (Typha)[1][2] är ett släkte i familjen kaveldunsväxter[1]. Släktet har 8–15 arter som förekommer i nästan hela världen. Släktet beskrevs först av Carl von Linné. I Sverige finns arterna bredkaveldun (T. latifolia) och smalkaveldun (T. angustifolia)</t>
-  </si>
-  <si>
     <t>Svinmålla</t>
   </si>
   <si>
@@ -238,9 +235,6 @@
     <t xml:space="preserve">Kummin har en mycket lång historia och kan spåras tillbaka till sumererna, som kallade kryddan gamun. De torkade frukterna (ofta felaktigt benämnda frön) används som krydda till exempelvis bröd, korv, ost och soppor. De används också för smaksättning av kryddat brännvin (akvavit). </t>
   </si>
   <si>
-    <t>Mycket lätt att förväxla med Vildpersilja som är mycket giftig. Undvik. Persilja är en tvåårig växt som blommar det andra året. Första året blir det bara en liten marknära bladrosett. Persilja är mycket rik på karoten (som omvandlas till A-vitamin i kroppen), B-vitaminer och C-vitamin samt järn och kalcium. Den är robust och tålig. Kan bli upp till 70 cm hög. Bladen är upprepat parflikiga. Det förekommer även framodlade sorter med starkt krusiga blad, "kruspersilja".</t>
-  </si>
-  <si>
     <t>Persilja</t>
   </si>
   <si>
@@ -253,9 +247,6 @@
     <t>Vildpersilja</t>
   </si>
   <si>
-    <t>Hela växten är mycket giftig, särskilt fröna. Förtäring medför kraftigt illamående, kräkning, diarré, stark salivavsöndring, muskelryckningar, smärta i buken och muskler, svårighet att röra på armarna och benen, sluddrande tal, dvala.[1] Många av följderna liknar dem hos epilepsi. Förgiftningar behandlas med magpumpning och därefter dryck.</t>
-  </si>
-  <si>
     <t>Selleri</t>
   </si>
   <si>
@@ -295,16 +286,10 @@
     <t>Anthriscus sylvestris</t>
   </si>
   <si>
-    <t>Svinmålla (Chenopodium album) är en ört. Den förekommer ofta, som "ogräs", i trädgårdsland och andra marker med bar jord. Bladen kan användas på samma sätt som spenat. Svinmålla är vanlig i norra Indien som gröda för mat.[1] I engelska texter kallas den ibland vid sitt hindi-namn bathua eller bathuwa.</t>
-  </si>
-  <si>
     <t>Körsbärskornell (Cornus mas) är en växtart i familjen kornellväxter och förekommer naturligt från centrala och sydöstra Europa till Kaukasus. Körsbärskornell är en lövfällande buske (4 meter hög) eller ett litet träd (8 meter), med bred och ganska låg krona. Bladen är äggrunda, med lång spets.</t>
   </si>
   <si>
     <t>Vildmorot (Daucus carota) är en art i familjen flockblommiga växter. I likhet med alla övriga arter i morotssläktet är växten tvåårig. Den förädlade moroten (D. carota sativa) klassas som en underart. Den förekommer i Eurasien och Nordafrika. Människan har spridit den till Amerika, där den blivit ett svårt ogräs. Till skillnad från den förädlade moroten har vildmoroten en tunn, träig pålrot - som dock ändå är ätlig.</t>
-  </si>
-  <si>
-    <t>Strätta (Angelica sylvestris) är en flerårig ört i släktet kvannar (Angelica) och familjen flockblommiga växter. Strättan är en mycket storvuxen ört med flikiga blad och stora vita eller rosa blomflockar, och förekommer i hela Europa och stora delar av Asien. Den återfinns framför allt på fuktig mark, bland annat på stränder och ängar samt på mänskligt störd mark som vägrenar och betesmarker. Roten har en aromatisk doft, och strättan har tidigare använts som färgväxt, i medicinen samt till örtte och mjöl.</t>
   </si>
   <si>
     <r>
@@ -363,13 +348,28 @@
     </r>
   </si>
   <si>
-    <t>Bockrot, vanlig bockrot eller backanis (Pimpinella saxifraga) är flerårig med en så kallad "månghövdad pålrot", det vill säga en kort kandelaberstam, uppburen av pålroten. Den växer allmänt på torra ängsbackar genom nästan hela Skandinavien. Roten är seg, smal och mycket djupgående, den har en brännande aromatisk smak och brukades förr som ett magstärkande och slemlösande läkemedel, till te mot hosta med mera. Den fanns med i den svenska farmakopén från 1775 fram till 1908 och såldes även på apoteken under de båda världskrigen. Ett extrakt av roten ingick bland annat i "Pimpinelladroppar" mot heshet och halsont</t>
-  </si>
-  <si>
     <t>Selleri (Apium graveolens) är en tvåårig, starkt doftande ört, som växer vilt i Europa, västra Asien och Nordafrika. Selleri har en lång historia som krydd- och medicinalväxt och den äts även som grönsak och rotfrukt. Det är främst roten, stjälken och fröna som används men även blad kan användas.</t>
   </si>
   <si>
     <t>Koriander har sitt ursprung i Sydeuropa och Asien. De torkade fröna har en kryddig, nötaktig behaglig smak. Bladen har en svårdefinierad aromatisk lukt och smak, som inte alla tycker om. Bladen används i asiatisk matlagning ungefär som man i Sverige använder persilja.</t>
+  </si>
+  <si>
+    <t>Strätta (Angelica sylvestris) är en flerårig ört i släktet kvannar (Angelica). Den återfinns framför allt på fuktig mark, bland annat på stränder och ängar samt på mänskligt störd mark som vägrenar och betesmarker. Roten har en aromatisk doft, och strättan har tidigare använts som färgväxt, i medicinen samt till örtte och mjöl.</t>
+  </si>
+  <si>
+    <t>Svinmålla (Chenopodium album) är en ört. Den förekommer ofta, som ogräs, i trädgårdsland och andra marker med bar jord. Bladen kan användas på samma sätt som spenat. Svinmålla är vanlig i norra Indien som gröda för mat. I engelska texter kallas den ibland vid sitt hindi-namn bathua eller bathuwa.</t>
+  </si>
+  <si>
+    <t>Bockrot, vanlig bockrot eller backanis (Pimpinella saxifraga) är flerårig. Den växer allmänt på torra ängsbackar genom nästan hela Skandinavien. Roten är seg, smal och mycket djupgående, den har en brännande aromatisk smak och brukades förr som ett magstärkande och slemlösande läkemedel, till te mot hosta med mera. Den fanns med i den svenska farmakopén från 1775 fram till 1908 och såldes även på apoteken under de båda världskrigen. Ett extrakt av roten ingick bland annat i Pimpinelladroppar mot heshet och halsont.</t>
+  </si>
+  <si>
+    <t>Hela växten är mycket giftig, särskilt fröna. Förtäring medför kraftigt illamående, kräkning, diarré, stark salivavsöndring, muskelryckningar, smärta i buken och muskler, svårighet att röra på armarna och benen, sluddrande tal, dvala. Många av följderna liknar dem hos epilepsi. Förgiftningar behandlas med magpumpning och därefter dryck.</t>
+  </si>
+  <si>
+    <t>Kaveldunsläktet (Typha) är ett släkte i familjen kaveldunsväxter. Släktet har 8–15 arter som förekommer i nästan hela världen. Släktet beskrevs först av Carl von Linné. I Sverige finns arterna bredkaveldun (T. latifolia) och smalkaveldun (T. angustifolia)</t>
+  </si>
+  <si>
+    <t>Mycket lätt att förväxla med Vildpersilja som är mycket giftig. Undvik. Persilja är en tvåårig växt som blommar det andra året. Första året blir det bara en liten marknära bladrosett. Persilja är mycket rik på karoten (som omvandlas till A-vitamin i kroppen), B-vitaminer och C-vitamin samt järn och kalcium. Den är robust och tålig. Kan bli upp till 70 cm hög. Bladen är upprepat parflikiga. Det förekommer även framodlade sorter med starkt krusiga blad, kruspersilja.</t>
   </si>
 </sst>
 </file>
@@ -1221,15 +1221,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1244,7 +1244,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1262,53 +1262,44 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>2</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="D3">
         <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1319,135 +1310,159 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>96</v>
       </c>
       <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="K4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5">
         <v>1</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
       <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="K6">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>82</v>
       </c>
       <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="K8">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="C9" t="s">
         <v>91</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
-      <c r="I9">
+      <c r="H9">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
         <v>1</v>
       </c>
       <c r="F10">
@@ -1457,293 +1472,302 @@
         <v>1</v>
       </c>
       <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D12">
-        <v>3</v>
-      </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="I12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="D13">
         <v>2</v>
       </c>
-      <c r="J13">
-        <v>3</v>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="D14">
-        <v>2</v>
-      </c>
-      <c r="K14">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="D15">
         <v>2</v>
       </c>
-      <c r="E15">
-        <v>1</v>
+      <c r="J15">
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="D16">
-        <v>3</v>
-      </c>
-      <c r="K16">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="K17">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="D18">
         <v>2</v>
       </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
+      <c r="K18">
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
       </c>
       <c r="F19">
         <v>1</v>
       </c>
       <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="I19">
-        <v>1</v>
-      </c>
-      <c r="L19">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>95</v>
+        <v>19</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="L20">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F21">
         <v>1</v>
       </c>
       <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="L21">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="D22">
         <v>2</v>
       </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="G22">
         <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D23">
-        <v>2</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23">
-        <v>1</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="I23">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="K23">
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="D24">
         <v>2</v>
       </c>
       <c r="K24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L24">
         <v>1</v>
@@ -1751,59 +1775,56 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="K25">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D26">
         <v>2</v>
       </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26">
-        <v>1</v>
-      </c>
-      <c r="H26">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="C27" t="s">
-        <v>98</v>
+        <v>34</v>
       </c>
       <c r="D27">
         <v>2</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -1814,19 +1835,16 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>82</v>
+        <v>31</v>
       </c>
       <c r="D28">
-        <v>2</v>
-      </c>
-      <c r="E28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -1836,60 +1854,54 @@
       </c>
       <c r="H28">
         <v>1</v>
-      </c>
-      <c r="L28">
-        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="D29">
         <v>2</v>
       </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-      <c r="L29">
-        <v>1</v>
+      <c r="E29">
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>88</v>
+        <v>13</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="E30">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
       </c>
       <c r="G30">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L30">
+    <sortCondition ref="A2:A30"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="C10" r:id="rId1" tooltip="Ogräs" display="https://sv.wikipedia.org/wiki/Ogr%C3%A4s" xr:uid="{20AF4F85-92C6-47E9-B9BE-D7E0DA55EC47}"/>
+    <hyperlink ref="C28" r:id="rId1" tooltip="Ogräs" display="https://sv.wikipedia.org/wiki/Ogr%C3%A4s" xr:uid="{20AF4F85-92C6-47E9-B9BE-D7E0DA55EC47}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Disclamer, Added more Plants
* Added disclamer text
		* Added more plants [total 50, pictures: 78]
</commit_message>
<xml_diff>
--- a/Assets/Data/Plants.xlsx
+++ b/Assets/Data/Plants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity Projects\GitHub\Edible Plants\Assets\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2905B09-C5AB-4D68-B3EA-142F1728C244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6AAF99-020A-424A-A005-9196287564D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28860" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plants" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="163">
   <si>
     <t>Latin Name</t>
   </si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>Mjölke</t>
-  </si>
-  <si>
-    <t>Mjölke finns i norra halvklotets tempererade områden. Den är vanlig längs banvallar, på hyggen och diken i hela Sverige, ända upp på kalfjället. På 1950-talet nådde den enligt en inventering i Jämtland 1 120 m, 2008 har den klättrat upp till 1 380 m. Oberoende undersökningar i Uralbergen, Alperna, Pyrenéerna och Jurabergen har visat liknande tendenser. Orsaken antas vara den globala uppvärmningen</t>
   </si>
   <si>
     <t>Typha</t>
@@ -388,6 +385,268 @@
   </si>
   <si>
     <t>Hundkäx (Anthriscus sylvestris) är en allmänt förekommande växt som tillhör släktet småkörvlar (Anthriscus). I Sverige förekommer hundkäx allmänt i hela landet och utgör den mest förekommande arten ur familjen flockblommiga växter. Stundtals går den till och med att återfinna ovanför trädgränsen, dock enbart tillfälligt. Hundkäx kan framförallt sammanblandas med spansk körvel (Myrrhis odorata), odört (Conium maculatum) samt vildpersilja (Aethusa cynapium).</t>
+  </si>
+  <si>
+    <t>Havtorn</t>
+  </si>
+  <si>
+    <t>Hippophaë rhamnoides</t>
+  </si>
+  <si>
+    <t>Oenothera glazioviana</t>
+  </si>
+  <si>
+    <t>Jättenattljus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mjölke finns i norra halvklotets tempererade områden. Den har många namn såsom rallarros, rävarumpa, praktdua samt mjölke eller mjölkört. Den är vanlig längs banvallar, på hyggen och diken i hela Sverige, ända upp på kalfjället. Alla delar av växten har brukats, små späda skott som sparris, bladen som sallad, spenat eller te. Brygg te på bladen som skärdas inna växten går io blom. Koka förväll eller rosta roten. Kaffesubstitut. Unga stjälkar har torkats och malts till mjöl. </t>
+  </si>
+  <si>
+    <t>Lathyrus linifolius</t>
+  </si>
+  <si>
+    <r>
+      <t>Gökärt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Fridlyst</t>
+  </si>
+  <si>
+    <t>Knölvial</t>
+  </si>
+  <si>
+    <t>Lathyrus tuberosus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I Sverige vanlig söder om Dalälven, mindre vanlig norr därom. Finns ej i Övre Norrland. Blomman är ätbar och således även kallad gökmat i vissa områden. Roten är näringsrik och kan bakas till nödbröd. I Skottland lär den ha tuggats rå, utan någon särskild matlagning. </t>
+  </si>
+  <si>
+    <t>I Sverige växer havtorn främst längs med östersjökusten, mest allmänt i Uppland. Den förekommer också på enstaka platser i Bohuslän, på Öland, i Skåne och i Upplands inland och längs Bottenviken i Norrbotten. Honplantorna producerar orangefärgade bär med en diameter av sex–nio millimeter, som är mjuka och saftiga och rika på C-vitamin 120 milligram C-vitamin per 100 gram bär.</t>
+  </si>
+  <si>
+    <t>Kråkvicker</t>
+  </si>
+  <si>
+    <t>Vicia cracca</t>
+  </si>
+  <si>
+    <t>Häckvicker växer ofta på relativt mager gräsmark, i häckar samt längs vägrenar. Den klänger normalt på annan vegeration. Kan möjligtvis blandas ihop med kråkvicker. Arterna skiljs åt genom att kråkvicker har mindre, mörkgrönare småblad och fler småblad per bladskaft. Dessutom har häckvicker färre blommor och ofta en något rödare variant av den violetta färgen.</t>
+  </si>
+  <si>
+    <t>Häckvicker</t>
+  </si>
+  <si>
+    <t>Vicia sepium</t>
+  </si>
+  <si>
+    <t>Vitklöver blommar från juni till september och är en av Nordens allmännaste växter. Vitklövern är den klöverart som lättast bildar genetiska missbildningar (mutationer) i bladen, vilka ger som resultat att bladet i stället för att bli tredelat blir delat på fyra, det vi kallar för fyrklöver. Vid växtfärgning kan vitklöverblommor användas för att med alun som betmedel färga ylle gult. Boskap samt människa kan använda blommorna som mat. Vitklöverblommor kan nyttjas som ingrediens i nödbröd.</t>
+  </si>
+  <si>
+    <t>Vitklöver</t>
+  </si>
+  <si>
+    <t>Trifolium repens</t>
+  </si>
+  <si>
+    <t>Rödklöver</t>
+  </si>
+  <si>
+    <t>Trifolium pratense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denna växt är vanlig på frisk jord i skogskanter, på ängar, vägkanter och öppen skog. Den klarar sig inte bra på gödslad jord. Skogsklövern har lågt betesvärde och betraktas närmast som ett ogräs av jordbrukare. </t>
+  </si>
+  <si>
+    <t>Trifolium medium</t>
+  </si>
+  <si>
+    <t>Skogsklöver</t>
+  </si>
+  <si>
+    <t>Jättenattljus (Oenothera glazioviana) är en art i familjen dunörtsväxter. Arten förekommer inte vild i den vanliga bemärkelsen utan har uppstått i Europa genom hybridisering av två odlade arter. Ingen av växterna i familjen betraktas som giftig. Hybriden är genetiskt stabil och räknas därför som en ny art. När blomman vissnar ersätts den med fröskida med värdefulla frön, vilket man kan extrahera den till naturmedelsoljan vars namn är Jättenattljusolja, fröna kallpressas. Den har i England odlats för sina ätliga rötter och i tyskland har skott ätits.</t>
+  </si>
+  <si>
+    <t>Knölvial (Lathyrus tuberosus) är en art i familjen ärtväxter. Arten förekommer i större delen av Europa, österut till Centralasien. Odlas ibland för sina ätliga rotknölar. Knölarna kallades i äldre tid jordnötter eller jordmöss, då de 3–4 centimeter långa knölarna liknar små möss, och smakar som kastanjer. Särskilt under 1800-talet ansågs knölvialens rotknölar som en läckerhet. Numera odlas arten oftare som prydnadsväxt.</t>
+  </si>
+  <si>
+    <r>
+      <t>Kråkvicker</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tranärt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> eller </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>fågelvicker</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vicia cracca</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) är en art i familjen ärtväxter som förekommer naturligt i stora delar av Eurasien, i Sverige är den vanlig överallt utom i fjälltrakterna. Arten har tidigare odlats som foderväxt i Sverige.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Rödklöver (Trifolium pratense L.) är en flerårig ört. Den är den mest odlade ärtväxten i Sverige, där den har odlats sedan 1700-talet, och används som numera ensilerad vallväxt. Färska blommor och småskurna blad kan användas i sallader. Den välsmakande nektarn kan sugas ut från blomman. Blommorna kan torkas och malas till mjöl. Detta har enligt Carl von Linné varit vanligt på Irland under nödår. </t>
+  </si>
+  <si>
+    <t>Cytisus scoparius</t>
+  </si>
+  <si>
+    <t>Harris</t>
+  </si>
+  <si>
+    <t>Den blir från 40 till 150 cm hög och blommar från maj till juni med orangegula blommor som växer med en till två blommor på cirka två cm långa skaft från bladvecken. Harris växer i form av en kvastlik buske med femkantiga gröna grenar utan tornar. Unga knoppar kan användas i sallad.Stora mängder har orsakat förgiftningar hos djur då den innehåller spartein och isospartein. Har använts som abortframkallande medel.</t>
+  </si>
+  <si>
+    <t>Häggmispel är en buske eller ett mindre träd, och blir upp till fem meter hög. Arten är ljuskrävande, men tål vind. Som förvildad hittas den ofta i skogsbryn, lövskogar, vägrenar och dungar i anslutning till gårdar. Till skillnad från flera andra arter i häggmispelsläktet, såsom svensk häggmispel, sen häggmispel och prakthäggmispel, är frukten inte att betrakta som smaklig.</t>
+  </si>
+  <si>
+    <t>Häggmispel</t>
+  </si>
+  <si>
+    <t>Amelanchier spicata</t>
+  </si>
+  <si>
+    <t>Crataegus</t>
+  </si>
+  <si>
+    <t>Hagtorn</t>
+  </si>
+  <si>
+    <t>Många arter och hybrider av hagtornar används som park- eller alléträd. Hagtorn används i Europa ofta som en häckväxt. Särskilt rosablommande kultivarer av rundhagtorn är populära i dessa sammanhang. Unga blad eller blommor kan torkas till te eller användas i sallader. Frukterna har används som mjölersättning. Torkade frukter som kaffesurregat.</t>
+  </si>
+  <si>
+    <t>Rönnbär</t>
+  </si>
+  <si>
+    <t>Sorbus aucuparia</t>
+  </si>
+  <si>
+    <t>Frukterna kallas rönnbär och är små äppelfrukter, med endast 2 eller 3 rum med mycket tunna, mjuka hinnväggar. De mogna rönnbären utgör den viktigaste vinterfödan för många fågelarter, till exempel sidensvans och trastar. Genom fåglarna sprids fröna, och kan då också hamna på tak, murar, bergväggar och uppe i kronorna på större träd. Eftersom rönnbären är beska och syrliga konsumeras de sällan av människor. Rönnbären används till rönnbärsgelé och till att krydda brännvin. På grund av den höga halten av vitamin C användes de mot skörbjugg. Rönnbären innehåller även naturliga antioxidanter i form av polyfenoler. Kyla gör att syrligheten mildras och därför brukar rönnbären plockas först efter första frostnatten. Unga blad ska kunna användas i sallader. Sorbitol kan fabrikframställas av bären.</t>
+  </si>
+  <si>
+    <t>Finnoxel</t>
+  </si>
+  <si>
+    <t>Finnoxeln är ett lågt träd, 4–5 m högt, ibland buskartat. Bladen är ludna på undersidan. Blommar i juni med gulvita starkt doftande blommor i klasar. Bären är centimeterstora och röda, smakar något surt. Träd med snarlika utseenden är fagerrönn (Sorbus meinchii) och avarönn (Sorbus teodori). Ska man använda oxelbär är finnoxeln att föredra. Torkade malda mjöl har använts i mjöl. Det har även kokats sirap, bryggts till öl och svagdricka. Torkade har de använts i soppor och välling. Mos och gele.</t>
+  </si>
+  <si>
+    <t>Sorbus hybrida</t>
+  </si>
+  <si>
+    <t>Sorbus intermedia</t>
+  </si>
+  <si>
+    <t>Svenskoxel</t>
+  </si>
+  <si>
+    <t>Oxeln uppkom i Sverige för mindre än 12 000 år sedan genom korsning av arter som kommit in från kontinenten efter istiden. Korsningen involverade två träd varav det ena var en tyskoxel (S. torminalis). Jämfört med rönnen har den något större blommor, större, avlånga frukter av mörkare, brunröd färg och mjöligare, sötaktigt fruktkött. Veden har en densitet på 0,6 vilket är det tyngsta och hårdaste träet i Sverige.</t>
+  </si>
+  <si>
+    <t>Vitoxel förekommer i nästan hela Europa. Beståndet i Norge och Sverige är introducerad för länge sedan och arten betraktas i Skandinavien som inhemsk art.</t>
+  </si>
+  <si>
+    <t>Sorbus aria</t>
+  </si>
+  <si>
+    <t>Vitoxel</t>
+  </si>
+  <si>
+    <t>Mispel</t>
+  </si>
+  <si>
+    <t>Mespilus germanica</t>
+  </si>
+  <si>
+    <t>Mispel (Mespilus germanica) är en art i familjen rosväxter. Det är ett lövträd med bred krona och ätliga frukter. Under medeltiden hade trädet större betydelse i Syd- och Centraleuropa och i England var mispel vanlig under 1600- och 1700-talet. Frukten liknar ett äpple men med långa utdragna foderflikar. Frukten är ätlig men anses inte så god då den innehåller mycket garvsyra. Kan mildras något efter frost.</t>
+  </si>
+  <si>
+    <t>Kvitten</t>
+  </si>
+  <si>
+    <t>Cydonia oblonga</t>
+  </si>
+  <si>
+    <t>RosenKvitten</t>
+  </si>
+  <si>
+    <t>Chaenomeles</t>
+  </si>
+  <si>
+    <t>Vanliga trädgårdsväxter. Släktet består av lövfällande buskar, eller i sällsynta fall små träd, ibland med tornar. Blad enkla, tandade. Frukterna är hård och sura och svårätna råa. De slemmiga fröna har används som handbalsam och hårinläggningsmedel. Frukterna kan användas till gele, vin, marmelad eller mos.</t>
+  </si>
+  <si>
+    <t>Kvitten (Cydonia oblonga) är ett lövfällande träd inom familjen rosväxter och ensam art i släktet Cydonia. Dess frukt är lik ett stort äpple, med fastare fruktkött som bland annat används till marmelad. Frukten kan ätas färsk (då måste man slå frukten innan man äter den. Slagen frigör saften. Man skär bitar lagom stora att tugga i. Bäst lyckas man om man håller frukten i sin ena hand och slår med en kavel lite hårt runt hela frukten med den andra) eller kokas till sylt, marmelad eller gelé. E att förväxla med den i Sverige mer vanliga Rosenkvitten.</t>
   </si>
 </sst>
 </file>
@@ -1238,10 +1497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,7 +1511,7 @@
     <col min="4" max="4" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1263,7 +1522,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1281,16 +1540,19 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1307,15 +1569,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1327,15 +1589,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
         <v>71</v>
       </c>
-      <c r="B4" t="s">
-        <v>72</v>
-      </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1344,7 +1606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1370,15 +1632,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -1393,41 +1655,41 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" t="s">
         <v>82</v>
       </c>
-      <c r="B7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B8" t="s">
-        <v>83</v>
-      </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1442,15 +1704,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -1468,16 +1730,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
         <v>66</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>67</v>
       </c>
-      <c r="C10" t="s">
-        <v>68</v>
-      </c>
       <c r="D10">
         <v>2</v>
       </c>
@@ -1497,7 +1759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1505,7 +1767,7 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>108</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1514,15 +1776,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1537,16 +1799,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" t="s">
         <v>102</v>
       </c>
-      <c r="B13" t="s">
-        <v>101</v>
-      </c>
-      <c r="C13" t="s">
-        <v>103</v>
-      </c>
       <c r="D13">
         <v>2</v>
       </c>
@@ -1554,16 +1816,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" t="s">
         <v>99</v>
       </c>
-      <c r="B14" t="s">
-        <v>98</v>
-      </c>
-      <c r="C14" t="s">
-        <v>100</v>
-      </c>
       <c r="D14">
         <v>2</v>
       </c>
@@ -1571,15 +1833,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" t="s">
         <v>75</v>
       </c>
-      <c r="B15" t="s">
-        <v>76</v>
-      </c>
       <c r="C15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -1591,15 +1853,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D16">
         <v>3</v>
@@ -1613,13 +1875,13 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -1630,13 +1892,13 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -1647,13 +1909,13 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -1676,13 +1938,13 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20">
         <v>2</v>
@@ -1739,13 +2001,13 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D23">
         <v>3</v>
@@ -1762,13 +2024,13 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D24">
         <v>2</v>
@@ -1791,13 +2053,13 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25">
         <v>3</v>
@@ -1808,13 +2070,13 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D26">
         <v>2</v>
@@ -1828,13 +2090,13 @@
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1845,13 +2107,13 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D28">
         <v>2</v>
@@ -1865,13 +2127,13 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D29">
         <v>2</v>
@@ -1888,13 +2150,13 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
         <v>31</v>
       </c>
-      <c r="B30" t="s">
-        <v>32</v>
-      </c>
       <c r="C30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -1911,13 +2173,13 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" t="s">
         <v>25</v>
       </c>
-      <c r="B31" t="s">
-        <v>26</v>
-      </c>
       <c r="C31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D31">
         <v>2</v>
@@ -1934,7 +2196,7 @@
         <v>12</v>
       </c>
       <c r="C32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -1947,6 +2209,368 @@
       </c>
       <c r="G32">
         <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" t="s">
+        <v>104</v>
+      </c>
+      <c r="C33" t="s">
+        <v>115</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" t="s">
+        <v>129</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B35" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>113</v>
+      </c>
+      <c r="B36" t="s">
+        <v>112</v>
+      </c>
+      <c r="C36" t="s">
+        <v>130</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>117</v>
+      </c>
+      <c r="B37" t="s">
+        <v>116</v>
+      </c>
+      <c r="C37" t="s">
+        <v>131</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>120</v>
+      </c>
+      <c r="B38" t="s">
+        <v>119</v>
+      </c>
+      <c r="C38" t="s">
+        <v>118</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>123</v>
+      </c>
+      <c r="B39" t="s">
+        <v>122</v>
+      </c>
+      <c r="C39" t="s">
+        <v>121</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>125</v>
+      </c>
+      <c r="B40" t="s">
+        <v>124</v>
+      </c>
+      <c r="C40" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>127</v>
+      </c>
+      <c r="B41" t="s">
+        <v>128</v>
+      </c>
+      <c r="C41" t="s">
+        <v>126</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B42" t="s">
+        <v>134</v>
+      </c>
+      <c r="C42" t="s">
+        <v>135</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B43" t="s">
+        <v>137</v>
+      </c>
+      <c r="C43" t="s">
+        <v>136</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B44" t="s">
+        <v>140</v>
+      </c>
+      <c r="C44" t="s">
+        <v>141</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B45" t="s">
+        <v>142</v>
+      </c>
+      <c r="C45" t="s">
+        <v>144</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B46" t="s">
+        <v>145</v>
+      </c>
+      <c r="C46" t="s">
+        <v>146</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B47" t="s">
+        <v>149</v>
+      </c>
+      <c r="C47" t="s">
+        <v>150</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>152</v>
+      </c>
+      <c r="B48" t="s">
+        <v>153</v>
+      </c>
+      <c r="C48" t="s">
+        <v>151</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>155</v>
+      </c>
+      <c r="B49" t="s">
+        <v>154</v>
+      </c>
+      <c r="C49" t="s">
+        <v>156</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>158</v>
+      </c>
+      <c r="B50" t="s">
+        <v>157</v>
+      </c>
+      <c r="C50" t="s">
+        <v>162</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>160</v>
+      </c>
+      <c r="B51" t="s">
+        <v>159</v>
+      </c>
+      <c r="C51" t="s">
+        <v>161</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+      <c r="J51">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1955,8 +2579,9 @@
   </sortState>
   <hyperlinks>
     <hyperlink ref="C30" r:id="rId1" tooltip="Ogräs" display="https://sv.wikipedia.org/wiki/Ogr%C3%A4s" xr:uid="{20AF4F85-92C6-47E9-B9BE-D7E0DA55EC47}"/>
+    <hyperlink ref="C41" r:id="rId2" location="Förklara_sammanhanget" tooltip="Wikipedia:Inledning och sammanhang" display="https://sv.wikipedia.org/wiki/Wikipedia:Inledning_och_sammanhang - Förklara_sammanhanget" xr:uid="{73307867-6B81-4F73-B236-36C8832E5A5D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Plants, fixed navigation
* Added 10 plants [total 80, pictures: 121]
		[Android Build: 102Mb] have 80 plants (121 images)
		[Android Build: 74Mb] Image compression 256 for pictures
		* Fixed navigation button size
</commit_message>
<xml_diff>
--- a/Assets/Data/Plants.xlsx
+++ b/Assets/Data/Plants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity Projects\GitHub\Edible Plants\Assets\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801ADECC-6A63-4C7F-9F0D-A06A0D82E137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BCAF6E-765D-4874-9A24-D42AB6956231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="256">
   <si>
     <t>Latin Name</t>
   </si>
@@ -884,6 +884,125 @@
   </si>
   <si>
     <t>Blodrot tillhör fingerörterna men avviker genom att blomman endast har 4 gula kronblad. Namnet kommer från den blodrödfärgade roten. Roten är besk och innehåller stora mängder garvsyra men har ändå ätits efter urlakning. Roten har använts som en medicinalväxt.</t>
+  </si>
+  <si>
+    <t>Surkörsbär</t>
+  </si>
+  <si>
+    <t>Surkörsbär (Prunus cerasus) är en art i familjen rosväxter. Arten förekommer förvildad i största delen av Europa. Anses fungera bättre till sylt, saft och vin eftersom bäret har starkare arom och hållbarhet än odlade varianter. Går att äta råa men kan vara ganska sura.</t>
+  </si>
+  <si>
+    <t>Prunus cerasus</t>
+  </si>
+  <si>
+    <t>Sötkörsbär eller fågelbär, Prunus avium, är en art i plommonsläktet inom familjen rosväxter. Arten förekommer naturligt i Europa. Det är träd som blir cirka 15–30 meter högt, och den art från vilken de flesta odlade kultivarer av körsbär tagits fram. Det finns i three main variteter såsom Bigarråer, vanlig sötkörsbär</t>
+  </si>
+  <si>
+    <t>Prunus avium</t>
+  </si>
+  <si>
+    <t>Sötkörsbär</t>
+  </si>
+  <si>
+    <t>Prunus padus</t>
+  </si>
+  <si>
+    <t>Hägg</t>
+  </si>
+  <si>
+    <t>Barken och frukterna är rika på amygdalin vilket bittermandelolja kan framställas ur. Bären är sträva ungefär som slånbär men är ätliga. Med fördel kokas saft eller vin på bäret. Kärnorna är svåra att skilja från bäret och används därför sällan till sylt.</t>
+  </si>
+  <si>
+    <t>Slån</t>
+  </si>
+  <si>
+    <t>Den får blå eller blåsvarta stenfrukter som kallas slånbär. Busken, som har vassa tornar, växer vilt i större delen av Europa. I Sverige är den vanlig i södra Sveriges kustlandskap. Bären innehåller garvsyra som ger dem en kärv och sur, nästan bitter smak. När temperaturen sjunker under noll grader omvandlas garvsyran, och slånbärens smak blir sötare och mindre sträv. Det fungerar utmärkt att imitera detta genom att lägga dem i frysen under 1–2 dygn. Bären har länge använts till att koka saft och vin. Bladen och blommorna kan användas till te. Veden är mycket hårt och har använts till sniderier. Barken till garvning av läder.</t>
+  </si>
+  <si>
+    <t>Prunus spinosa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brudbröd är lätt igenkänd på de starka och sega rötternas tjocka, kulformiga uppsvällningar, hårda men dock något köttiga knölar, som magasinerar vatten för torra perioder. Brudbrödet är Älgörtens närmaste släkting. Rötterna kan kokas och ätas som potatis. </t>
+  </si>
+  <si>
+    <t>Filipendula vulgaris</t>
+  </si>
+  <si>
+    <t>Brudbröd</t>
+  </si>
+  <si>
+    <t>Älggräs</t>
+  </si>
+  <si>
+    <t>Filipendula ulmaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Älggräs (Filipendula ulmaria L.), älgört, är en ört i släktet älggräs i familjen rosväxter. Den högväxta arten har små vita och starkt doftande blommor. Blommor och blad innehåller acetylsalicylsyra, och arten har använts både i medicinskt syfte och som smaksättning av drycker. Den växer i fuktiga marker såsom diken och skuggiga stränder. Kan finnas i mängder på ängar. Blommor kan användas som te och fungerar mot huvudvärk då den innehåller salicylsyra. </t>
+  </si>
+  <si>
+    <t>Medicinsk</t>
+  </si>
+  <si>
+    <t>Huvudvärk</t>
+  </si>
+  <si>
+    <t>Ribes alpinum</t>
+  </si>
+  <si>
+    <t>Måbär</t>
+  </si>
+  <si>
+    <t>Måbärsbusken är ganska allmän i lundar och skogsbackar, i synnerhet i östra Götaland och Svealand, men finns glest utbredd från Skåne till mellersta Norrland. Han och honblommor sitter på skilda buskar. Liknar vinbär och bären är ätbara, söta men lite fadda i smaken.</t>
+  </si>
+  <si>
+    <t>Röda vinbär</t>
+  </si>
+  <si>
+    <t>Ribes rubrum</t>
+  </si>
+  <si>
+    <t>Ribes nigrum</t>
+  </si>
+  <si>
+    <t>Svarta vinbär</t>
+  </si>
+  <si>
+    <t>Röda vinbär är ett samlingsnamn för trädgårdsvinbär (Ribes rubrum) och skogsvinbär (Ribes spicatum). Ibland har bägge dessa ansetts vara underarter av samma huvudart. Förvildade trädgårdsvinbär kan förekomma i samma områden som skogsvinbär. Vita vinbär är en variant. Bären är sura och kan ätas råa eller kokas till sylt, saft eller gelé. Bären innehåller stora mängder pektin och kan därför användas tillsammans med andra bär för att skapa gelé.</t>
+  </si>
+  <si>
+    <t>Svarta vinbär eller svartvinbär (Ribes nigrum) är en växt som tillhör Vinbärssläktet och familjen ripsväxter. En gammal synonym är tistron. Bären är mycket rika på C-vitamin och anses nyttigare och godare än det röda vinbäret. Används till sylt, saft, vin eller gelé. Bladen kan användas som fläderblommor eller till te och gurkinläggningar.</t>
+  </si>
+  <si>
+    <t>Krusbär</t>
+  </si>
+  <si>
+    <t>Ribes uva-crispa</t>
+  </si>
+  <si>
+    <r>
+      <t>Krusbär (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ribes uva-crispa</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) är namnet både på en buske och dess bär. Den dök förmodligen upp i sverige på 1500-talet. Busken har taggiga grenar. Bären kan drabbas av krusbärsmjöldaggen som är en parasitsvamp som täcker in bäret i en brunt ludd och gör den oätlig. Bären används till sylt, saft, gelé eller vin.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1757,11 +1876,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N71"/>
+  <dimension ref="A1:O81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F63" sqref="F63"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1772,9 +1891,10 @@
     <col min="4" max="4" width="10.42578125" customWidth="1"/>
     <col min="11" max="11" width="15.42578125" customWidth="1"/>
     <col min="12" max="12" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1817,8 +1937,11 @@
       <c r="N1" s="2" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -1835,7 +1958,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -1855,7 +1978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -1872,7 +1995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1898,7 +2021,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1921,7 +2044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -1947,7 +2070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -1970,7 +2093,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -1996,7 +2119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>63</v>
       </c>
@@ -2025,7 +2148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -2042,7 +2165,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -2065,7 +2188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>98</v>
       </c>
@@ -2082,7 +2205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>95</v>
       </c>
@@ -2099,7 +2222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>72</v>
       </c>
@@ -2119,7 +2242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -3135,7 +3258,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>203</v>
       </c>
@@ -3155,7 +3278,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>204</v>
       </c>
@@ -3172,7 +3295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>209</v>
       </c>
@@ -3189,7 +3312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>212</v>
       </c>
@@ -3206,7 +3329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>215</v>
       </c>
@@ -3223,7 +3346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>217</v>
       </c>
@@ -3240,7 +3363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>221</v>
       </c>
@@ -3255,6 +3378,224 @@
       </c>
       <c r="N71">
         <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>226</v>
+      </c>
+      <c r="B72" t="s">
+        <v>224</v>
+      </c>
+      <c r="C72" t="s">
+        <v>225</v>
+      </c>
+      <c r="D72">
+        <v>2</v>
+      </c>
+      <c r="J72">
+        <v>1</v>
+      </c>
+      <c r="L72">
+        <v>1</v>
+      </c>
+      <c r="N72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B73" t="s">
+        <v>229</v>
+      </c>
+      <c r="C73" t="s">
+        <v>227</v>
+      </c>
+      <c r="D73">
+        <v>2</v>
+      </c>
+      <c r="J73">
+        <v>1</v>
+      </c>
+      <c r="N73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B74" t="s">
+        <v>231</v>
+      </c>
+      <c r="C74" t="s">
+        <v>232</v>
+      </c>
+      <c r="D74">
+        <v>2</v>
+      </c>
+      <c r="J74">
+        <v>1</v>
+      </c>
+      <c r="N74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B75" t="s">
+        <v>233</v>
+      </c>
+      <c r="C75" t="s">
+        <v>234</v>
+      </c>
+      <c r="D75">
+        <v>2</v>
+      </c>
+      <c r="G75">
+        <v>2</v>
+      </c>
+      <c r="H75">
+        <v>2</v>
+      </c>
+      <c r="J75">
+        <v>1</v>
+      </c>
+      <c r="N75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B76" t="s">
+        <v>238</v>
+      </c>
+      <c r="C76" t="s">
+        <v>236</v>
+      </c>
+      <c r="D76">
+        <v>2</v>
+      </c>
+      <c r="E76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>240</v>
+      </c>
+      <c r="B77" t="s">
+        <v>239</v>
+      </c>
+      <c r="C77" t="s">
+        <v>241</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="H77">
+        <v>2</v>
+      </c>
+      <c r="O77" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B78" t="s">
+        <v>245</v>
+      </c>
+      <c r="C78" t="s">
+        <v>246</v>
+      </c>
+      <c r="D78">
+        <v>2</v>
+      </c>
+      <c r="J78">
+        <v>1</v>
+      </c>
+      <c r="N78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>248</v>
+      </c>
+      <c r="B79" t="s">
+        <v>247</v>
+      </c>
+      <c r="C79" t="s">
+        <v>251</v>
+      </c>
+      <c r="D79">
+        <v>2</v>
+      </c>
+      <c r="J79">
+        <v>1</v>
+      </c>
+      <c r="L79">
+        <v>1</v>
+      </c>
+      <c r="N79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>249</v>
+      </c>
+      <c r="B80" t="s">
+        <v>250</v>
+      </c>
+      <c r="C80" t="s">
+        <v>252</v>
+      </c>
+      <c r="D80">
+        <v>2</v>
+      </c>
+      <c r="G80">
+        <v>2</v>
+      </c>
+      <c r="J80">
+        <v>1</v>
+      </c>
+      <c r="L80">
+        <v>1</v>
+      </c>
+      <c r="N80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>254</v>
+      </c>
+      <c r="B81" t="s">
+        <v>253</v>
+      </c>
+      <c r="C81" t="s">
+        <v>255</v>
+      </c>
+      <c r="D81">
+        <v>2</v>
+      </c>
+      <c r="J81">
+        <v>1</v>
+      </c>
+      <c r="L81">
+        <v>1</v>
+      </c>
+      <c r="N81">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Isssue fixed, Information Page added, military
* Fixed build issue install on phone not enough storage space
		* Added Information page
		* Added info of millitary top plants
</commit_message>
<xml_diff>
--- a/Assets/Data/Plants.xlsx
+++ b/Assets/Data/Plants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity Projects\GitHub\Edible Plants\Assets\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FBEFA9-5431-4A9E-99E7-0029BEA1CDB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF718AE-1845-48EA-B8D3-3559A1FF81E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="319">
   <si>
     <t>Latin Name</t>
   </si>
@@ -619,9 +619,6 @@
     <t>Vanliga trädgårdsväxter. Släktet består av lövfällande buskar, eller i sällsynta fall små träd, ibland med tornar. Blad enkla, tandade. Frukterna är hård och sura och svårätna råa. De slemmiga fröna har används som handbalsam och hårinläggningsmedel. Frukterna kan användas till gele, vin, marmelad eller mos.</t>
   </si>
   <si>
-    <t>Kvitten (Cydonia oblonga) är ett lövfällande träd inom familjen rosväxter och ensam art i släktet Cydonia. Dess frukt är lik ett stort äpple, med fastare fruktkött som bland annat används till marmelad. Frukten kan ätas färsk (då måste man slå frukten innan man äter den. Slagen frigör saften. Man skär bitar lagom stora att tugga i. Bäst lyckas man om man håller frukten i sin ena hand och slår med en kavel lite hårt runt hela frukten med den andra) eller kokas till sylt, marmelad eller gelé. E att förväxla med den i Sverige mer vanliga Rosenkvitten.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mjölke finns i norra halvklotets tempererade områden. Den har många namn såsom rallarros, rävarumpa, praktdua samt mjölke eller mjölkört. Den är vanlig längs banvallar, på hyggen och diken i hela Sverige, ända upp på kalfjället. Alla delar av växten har brukats. Små späda skott som sparris, bladen som sallad, spenat eller te. Te kan bryggas på bladen om de skärdas innan växten går i blom. Roten kan ätas efter kokning eller förvällning. Rostad rot har använts som kaffesubstitut. Unga stjälkar har torkats och malts till mjöl. </t>
   </si>
   <si>
@@ -866,9 +863,6 @@
   </si>
   <si>
     <t>Prunus domestica_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nyponros (Rosa dumalis) är en rosbuske, som kan växa sig tre meter hög. Den förväxlas lätt med stenros. Taggarna är tämligen grova och bakåtböjda. Nyponen är kala och ganska mjuka. Nyponrosen är den vanliga vildväxande rosarten i Sverige och är allmän från Skåne till Ångermanland. </t>
   </si>
   <si>
     <t>Blodrot tillhör fingerörterna men avviker genom att blomman endast har 4 gula kronblad. Namnet kommer från den blodrödfärgade roten. Roten är besk och innehåller stora mängder garvsyra men har ändå ätits efter urlakning. Roten har använts som en medicinalväxt.</t>
@@ -1293,6 +1287,15 @@
   </si>
   <si>
     <t>Skörbjuggsört (Cochlearia officinalis) är en två- eller flerårig ört inom släktet skörbjuggsörter och familjen korsblommiga växter. Underarten vanlig skörbjuggsört, ssp. officinalis, är vanlig på kustnära, öppen, stenig eller grusig mark och kan påträffas på exempelvis havsstrandängar, klippor, tångvallar och fågelberg. Dess utbredning i Norden är hela Norges kust, Sveriges västkust och del av östkust. Små blad kan ätas som sallad och har en senapslikanande smak och innehåller en del C-vitamin. Blad och stjälkar kan kokas till soppa. Förr konserverades örten och såldes som finnmarkskål.</t>
+  </si>
+  <si>
+    <t>Kvitten (Cydonia oblonga) är ett lövfällande träd inom familjen rosväxter och ensam art i släktet Cydonia. Dess frukt är lik ett stort äpple, med fastare fruktkött som bland annat används till marmelad. Frukten kan ätas färsk (då måste man slå frukten innan man äter den. Slagen frigör saften. Man skär bitar lagom stora att tugga i. Bäst lyckas man om man håller frukten i sin ena hand och slår med en kavel lite hårt runt hela frukten med den andra) eller kokas till sylt, marmelad eller gelé. Ej att förväxla med den i Sverige mer vanliga Rosenkvitten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nyponros (Rosa dumalis) är en rosbuske, som kan växa sig tre meter hög. Den förväxlas lätt med stenros. Taggarna är tämligen grova och bakåtböjda. Nyponen är kala och ganska mjuka. Nyponrosen är den vanligaste vildväxande rosarten i Sverige och är allmän från Skåne till Ångermanland. </t>
+  </si>
+  <si>
+    <t>Army</t>
   </si>
 </sst>
 </file>
@@ -2166,11 +2169,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O101"/>
+  <dimension ref="A1:P101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I82" sqref="I82"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2184,7 +2187,7 @@
     <col min="15" max="15" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="2" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2195,7 +2198,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -2216,22 +2219,25 @@
         <v>35</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -2248,7 +2254,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -2268,7 +2274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -2285,7 +2291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2311,7 +2317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -2334,7 +2340,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -2360,7 +2366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>80</v>
       </c>
@@ -2383,7 +2389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -2409,7 +2415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -2438,7 +2444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -2446,7 +2452,7 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -2454,8 +2460,11 @@
       <c r="E11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -2478,7 +2487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>97</v>
       </c>
@@ -2486,7 +2495,7 @@
         <v>96</v>
       </c>
       <c r="C13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -2495,7 +2504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>94</v>
       </c>
@@ -2512,7 +2521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>71</v>
       </c>
@@ -2532,7 +2541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -2869,13 +2878,13 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B32" t="s">
+        <v>162</v>
+      </c>
+      <c r="C32" t="s">
         <v>164</v>
-      </c>
-      <c r="B32" t="s">
-        <v>163</v>
-      </c>
-      <c r="C32" t="s">
-        <v>165</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -2895,7 +2904,7 @@
         <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -3107,7 +3116,7 @@
         <v>127</v>
       </c>
       <c r="C43" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D43">
         <v>2</v>
@@ -3173,7 +3182,7 @@
         <v>134</v>
       </c>
       <c r="C46" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D46">
         <v>1</v>
@@ -3273,7 +3282,7 @@
         <v>148</v>
       </c>
       <c r="C51" t="s">
-        <v>153</v>
+        <v>316</v>
       </c>
       <c r="D51">
         <v>2</v>
@@ -3307,13 +3316,13 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>157</v>
+      </c>
+      <c r="B53" t="s">
+        <v>156</v>
+      </c>
+      <c r="C53" t="s">
         <v>158</v>
-      </c>
-      <c r="B53" t="s">
-        <v>157</v>
-      </c>
-      <c r="C53" t="s">
-        <v>159</v>
       </c>
       <c r="D53">
         <v>2</v>
@@ -3327,13 +3336,13 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B54" t="s">
+        <v>165</v>
+      </c>
+      <c r="C54" t="s">
         <v>166</v>
-      </c>
-      <c r="C54" t="s">
-        <v>167</v>
       </c>
       <c r="D54">
         <v>2</v>
@@ -3350,13 +3359,13 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>168</v>
+      </c>
+      <c r="B55" t="s">
+        <v>170</v>
+      </c>
+      <c r="C55" t="s">
         <v>169</v>
-      </c>
-      <c r="B55" t="s">
-        <v>171</v>
-      </c>
-      <c r="C55" t="s">
-        <v>170</v>
       </c>
       <c r="D55">
         <v>2</v>
@@ -3370,13 +3379,13 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B56" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C56" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -3390,13 +3399,13 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B57" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C57" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D57">
         <v>2</v>
@@ -3416,13 +3425,13 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B58" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C58" t="s">
-        <v>218</v>
+        <v>317</v>
       </c>
       <c r="D58">
         <v>2</v>
@@ -3439,13 +3448,13 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B59" t="s">
+        <v>179</v>
+      </c>
+      <c r="C59" t="s">
         <v>180</v>
-      </c>
-      <c r="C59" t="s">
-        <v>181</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -3459,13 +3468,13 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>183</v>
+      </c>
+      <c r="B60" t="s">
+        <v>182</v>
+      </c>
+      <c r="C60" t="s">
         <v>184</v>
-      </c>
-      <c r="B60" t="s">
-        <v>183</v>
-      </c>
-      <c r="C60" t="s">
-        <v>185</v>
       </c>
       <c r="D60">
         <v>2</v>
@@ -3479,13 +3488,13 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B61" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C61" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D61">
         <v>2</v>
@@ -3496,13 +3505,13 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B62" t="s">
+        <v>187</v>
+      </c>
+      <c r="C62" t="s">
         <v>188</v>
-      </c>
-      <c r="C62" t="s">
-        <v>189</v>
       </c>
       <c r="D62">
         <v>2</v>
@@ -3513,13 +3522,13 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>191</v>
+      </c>
+      <c r="B63" t="s">
+        <v>190</v>
+      </c>
+      <c r="C63" t="s">
         <v>192</v>
-      </c>
-      <c r="B63" t="s">
-        <v>191</v>
-      </c>
-      <c r="C63" t="s">
-        <v>193</v>
       </c>
       <c r="D63">
         <v>2</v>
@@ -3530,13 +3539,13 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B64" t="s">
+        <v>193</v>
+      </c>
+      <c r="C64" t="s">
         <v>194</v>
-      </c>
-      <c r="C64" t="s">
-        <v>195</v>
       </c>
       <c r="D64">
         <v>2</v>
@@ -3550,13 +3559,13 @@
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B65" t="s">
+        <v>196</v>
+      </c>
+      <c r="C65" t="s">
         <v>197</v>
-      </c>
-      <c r="C65" t="s">
-        <v>198</v>
       </c>
       <c r="D65">
         <v>2</v>
@@ -3570,13 +3579,13 @@
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>199</v>
+      </c>
+      <c r="B66" t="s">
         <v>200</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
         <v>201</v>
-      </c>
-      <c r="C66" t="s">
-        <v>202</v>
       </c>
       <c r="D66">
         <v>2</v>
@@ -3587,13 +3596,13 @@
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B67" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C67" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D67">
         <v>1</v>
@@ -3604,13 +3613,13 @@
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B68" t="s">
+        <v>205</v>
+      </c>
+      <c r="C68" t="s">
         <v>206</v>
-      </c>
-      <c r="C68" t="s">
-        <v>207</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -3621,13 +3630,13 @@
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B69" t="s">
+        <v>208</v>
+      </c>
+      <c r="C69" t="s">
         <v>209</v>
-      </c>
-      <c r="C69" t="s">
-        <v>210</v>
       </c>
       <c r="D69">
         <v>2</v>
@@ -3638,13 +3647,13 @@
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>212</v>
+      </c>
+      <c r="B70" t="s">
         <v>213</v>
       </c>
-      <c r="B70" t="s">
-        <v>214</v>
-      </c>
       <c r="C70" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D70">
         <v>2</v>
@@ -3658,13 +3667,13 @@
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B71" t="s">
+        <v>214</v>
+      </c>
+      <c r="C71" t="s">
         <v>215</v>
-      </c>
-      <c r="C71" t="s">
-        <v>216</v>
       </c>
       <c r="D71">
         <v>2</v>
@@ -3678,13 +3687,13 @@
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B72" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C72" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D72">
         <v>2</v>
@@ -3701,13 +3710,13 @@
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B73" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C73" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D73">
         <v>2</v>
@@ -3721,13 +3730,13 @@
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>224</v>
+      </c>
+      <c r="B74" t="s">
+        <v>225</v>
+      </c>
+      <c r="C74" t="s">
         <v>226</v>
-      </c>
-      <c r="B74" t="s">
-        <v>227</v>
-      </c>
-      <c r="C74" t="s">
-        <v>228</v>
       </c>
       <c r="D74">
         <v>2</v>
@@ -3741,13 +3750,13 @@
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B75" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C75" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D75">
         <v>2</v>
@@ -3767,13 +3776,13 @@
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B76" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C76" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D76">
         <v>2</v>
@@ -3784,33 +3793,33 @@
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B77" t="s">
+        <v>233</v>
+      </c>
+      <c r="C77" t="s">
         <v>235</v>
       </c>
-      <c r="C77" t="s">
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="H77">
+        <v>2</v>
+      </c>
+      <c r="O77" t="s">
         <v>237</v>
-      </c>
-      <c r="D77">
-        <v>1</v>
-      </c>
-      <c r="H77">
-        <v>2</v>
-      </c>
-      <c r="O77" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>238</v>
+      </c>
+      <c r="B78" t="s">
+        <v>239</v>
+      </c>
+      <c r="C78" t="s">
         <v>240</v>
-      </c>
-      <c r="B78" t="s">
-        <v>241</v>
-      </c>
-      <c r="C78" t="s">
-        <v>242</v>
       </c>
       <c r="D78">
         <v>2</v>
@@ -3824,13 +3833,13 @@
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B79" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C79" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D79">
         <v>2</v>
@@ -3847,13 +3856,13 @@
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B80" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C80" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D80">
         <v>2</v>
@@ -3873,13 +3882,13 @@
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B81" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C81" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D81">
         <v>2</v>
@@ -3896,13 +3905,13 @@
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B82" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C82" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D82">
         <v>2</v>
@@ -3916,13 +3925,13 @@
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>256</v>
+      </c>
+      <c r="B83" t="s">
+        <v>257</v>
+      </c>
+      <c r="C83" t="s">
         <v>258</v>
-      </c>
-      <c r="B83" t="s">
-        <v>259</v>
-      </c>
-      <c r="C83" t="s">
-        <v>260</v>
       </c>
       <c r="D83">
         <v>2</v>
@@ -3936,13 +3945,13 @@
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B84" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C84" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D84">
         <v>2</v>
@@ -3953,13 +3962,13 @@
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B85" t="s">
+        <v>260</v>
+      </c>
+      <c r="C85" t="s">
         <v>262</v>
-      </c>
-      <c r="C85" t="s">
-        <v>264</v>
       </c>
       <c r="D85">
         <v>2</v>
@@ -3970,13 +3979,13 @@
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B86" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C86" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D86">
         <v>1</v>
@@ -3990,13 +3999,13 @@
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B87" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C87" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D87">
         <v>2</v>
@@ -4007,45 +4016,45 @@
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>270</v>
+      </c>
+      <c r="B88" t="s">
+        <v>269</v>
+      </c>
+      <c r="C88" t="s">
         <v>272</v>
       </c>
-      <c r="B88" t="s">
+      <c r="D88">
+        <v>2</v>
+      </c>
+      <c r="E88">
+        <v>2</v>
+      </c>
+      <c r="F88">
+        <v>1</v>
+      </c>
+      <c r="G88">
+        <v>1</v>
+      </c>
+      <c r="H88">
+        <v>1</v>
+      </c>
+      <c r="I88">
+        <v>1</v>
+      </c>
+      <c r="O88" t="s">
         <v>271</v>
-      </c>
-      <c r="C88" t="s">
-        <v>274</v>
-      </c>
-      <c r="D88">
-        <v>2</v>
-      </c>
-      <c r="E88">
-        <v>2</v>
-      </c>
-      <c r="F88">
-        <v>1</v>
-      </c>
-      <c r="G88">
-        <v>1</v>
-      </c>
-      <c r="H88">
-        <v>1</v>
-      </c>
-      <c r="I88">
-        <v>1</v>
-      </c>
-      <c r="O88" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B89" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C89" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D89">
         <v>2</v>
@@ -4068,13 +4077,13 @@
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B90" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C90" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D90">
         <v>2</v>
@@ -4091,13 +4100,13 @@
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B91" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C91" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D91">
         <v>2</v>
@@ -4111,13 +4120,13 @@
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B92" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C92" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D92">
         <v>2</v>
@@ -4131,13 +4140,13 @@
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>286</v>
+      </c>
+      <c r="B93" t="s">
+        <v>287</v>
+      </c>
+      <c r="C93" t="s">
         <v>288</v>
-      </c>
-      <c r="B93" t="s">
-        <v>289</v>
-      </c>
-      <c r="C93" t="s">
-        <v>290</v>
       </c>
       <c r="D93">
         <v>2</v>
@@ -4151,30 +4160,30 @@
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B94" t="s">
+        <v>290</v>
+      </c>
+      <c r="C94" t="s">
         <v>292</v>
       </c>
-      <c r="C94" t="s">
-        <v>294</v>
-      </c>
       <c r="D94">
         <v>2</v>
       </c>
       <c r="O94" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B95" t="s">
+        <v>293</v>
+      </c>
+      <c r="C95" t="s">
         <v>295</v>
-      </c>
-      <c r="C95" t="s">
-        <v>297</v>
       </c>
       <c r="D95">
         <v>2</v>
@@ -4185,13 +4194,13 @@
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B96" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C96" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D96">
         <v>1</v>
@@ -4202,13 +4211,13 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B97" t="s">
+        <v>298</v>
+      </c>
+      <c r="C97" t="s">
         <v>300</v>
-      </c>
-      <c r="C97" t="s">
-        <v>302</v>
       </c>
       <c r="D97">
         <v>1</v>
@@ -4225,13 +4234,13 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B98" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C98" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D98">
         <v>2</v>
@@ -4242,13 +4251,13 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B99" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C99" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D99">
         <v>1</v>
@@ -4262,13 +4271,13 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B100" t="s">
+        <v>307</v>
+      </c>
+      <c r="C100" t="s">
         <v>309</v>
-      </c>
-      <c r="C100" t="s">
-        <v>311</v>
       </c>
       <c r="D100">
         <v>2</v>
@@ -4285,13 +4294,13 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B101" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C101" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D101">
         <v>2</v>

</xml_diff>

<commit_message>
Images in Information versitiled
* Fixed images and text creation in information pages. Can now integrate pictures.
</commit_message>
<xml_diff>
--- a/Assets/Data/Plants.xlsx
+++ b/Assets/Data/Plants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity Projects\GitHub\Edible Plants\Assets\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F835DB4A-E982-4B9E-8AA1-4AFDC15FE64F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE0AFB8-C9E4-4812-A50D-EA23B08E3AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="399">
   <si>
     <t>Latin Name</t>
   </si>
@@ -266,9 +266,6 @@
   </si>
   <si>
     <t>Körsbärskornell (Cornus mas) är en växtart i familjen kornellväxter och förekommer naturligt från centrala och sydöstra Europa till Kaukasus. Körsbärskornell är en lövfällande buske (4 meter hög) eller ett litet träd (8 meter), med bred och ganska låg krona. Bladen är äggrunda, med lång spets.</t>
-  </si>
-  <si>
-    <t>Vildmorot (Daucus carota) är en art i familjen flockblommiga växter. I likhet med alla övriga arter i morotssläktet är växten tvåårig. Den förädlade moroten (D. carota sativa) klassas som en underart. Den förekommer i Eurasien och Nordafrika. Människan har spridit den till Amerika, där den blivit ett svårt ogräs. Till skillnad från den förädlade moroten har vildmoroten en tunn, träig pålrot - som dock ändå är ätlig.</t>
   </si>
   <si>
     <r>
@@ -634,9 +631,6 @@
     <t>Tree</t>
   </si>
   <si>
-    <t xml:space="preserve">1=Toxic,       2=Förväxl,   4=PartToxic   Avoid             </t>
-  </si>
-  <si>
     <t>Brännässla (Urtica dioica) är en art i familjen nässelväxter. Arten är allmän över hela Nordeuropa, men förekommer även i övriga Europa, Asien, Nordafrika och Nordamerika. Nässlorna växer i näringsrik jord och lagrar in nitrater vilket gör att vissa anser att man ej bör äta för mycket utav dem. Blad och skott hos unga plantor gör sig bäst efter kokning eller förvällning. Små plantor ska även gå att ätas råa. De kan även blandas i när man gör bröd. Stammen kan användas till att göra rep. Etternässlan kan användas på samma sätt.</t>
   </si>
   <si>
@@ -686,9 +680,6 @@
   </si>
   <si>
     <t>Rosa dumalis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nypon växer på nyponbuskar som är olika varianter av rosor. Nypon är mycket nyttiga då de innehåller stora mängder C-vitamin. Det finns många olike varianter av nypon men alla kan användas likvärdigt. Nyponte görs genom att koka frukterna i vatten och silar av. Det går även bra att koka marmelad, göra sylt eller soppa på dem men kärna då ur dem ordentligt. </t>
   </si>
   <si>
     <t>Daggkåpa</t>
@@ -869,9 +860,6 @@
   </si>
   <si>
     <t>Prunus cerasus</t>
-  </si>
-  <si>
-    <t>Sötkörsbär eller fågelbär, Prunus avium, är en art i plommonsläktet inom familjen rosväxter. Arten förekommer naturligt i Europa. Det är träd som blir cirka 15–30 meter högt, och den art från vilken de flesta odlade kultivarer av körsbär tagits fram. Det finns i three main variteter såsom Bigarråer, vanlig sötkörsbär</t>
   </si>
   <si>
     <t>Prunus avium</t>
@@ -1439,9 +1427,6 @@
     <t>Islandslav</t>
   </si>
   <si>
-    <t>Cetmria islandica</t>
-  </si>
-  <si>
     <t>Allmän i hela landet. Växer bland mossa och andra lavar i glesa skogar och hällmarker. Buskformig, löst tuvad. 1 torrt tillstånd grågrön till brungrön, i fuktigt tillstånd grön¬ aktig. Måste urlakas. Hela växten används.</t>
   </si>
   <si>
@@ -1533,6 +1518,24 @@
   </si>
   <si>
     <t>Vanlig i hela landet. Tallskogar är torra områden med lavar, lingon och ljung som markvegetation. Hos tallen är det främst barren som du använder. Av dessa kan du göra en god och vitaminrik dryck. Den äldre, hårda barken skrapas av intill det ljusgröna, tunna skiktet (innerbarken). Tidsödande. Bereds på samma sätt som ungbark. Förr i tiden när det var missväxt och svält var det vanligt att man blandade denna bark i brödet.</t>
+  </si>
+  <si>
+    <t>Sötkörsbär eller fågelbär, Prunus avium, är en art i plommonsläktet inom familjen rosväxter. Arten förekommer naturligt i Europa. Det är träd som blir cirka 15–30 meter högt, och den art från vilken de flesta odlade kultivarer av körsbär tagits fram. Det finns i tre variteter såsom Bigarråer, vanlig sötkörsbär och hjärtkörsbär.</t>
+  </si>
+  <si>
+    <t>Cetraria islandica</t>
+  </si>
+  <si>
+    <t>Lav Fungi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1=Toxic,       2=Förväxl,   4=PartToxic   Avoid             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nypon växer på nyponbuskar som är olika varianter av rosor. Nypon är mycket nyttiga då de innehåller stora mängder C-vitamin. Det finns många olika varianter av nypon men de kan användas likvärdigt. Nyponte görs genom att koka frukterna i vatten som man sedan silar av. Det går även bra att koka soppa och marmelad eller att göra sylt på dem, men kärna då ur dem ordentligt. </t>
+  </si>
+  <si>
+    <t>Vildmorot (Daucus carota) är en art i familjen flockblommiga växter. I likhet med alla övriga arter i morotssläktet är växten tvåårig. Den förädlade moroten (D. carota sativa) klassas som en underart. Den förekommer i Eurasien och Nordafrika. Människan har spridit den till Amerika, där den blivit ett svårt ogräs. Till skillnad från den förädlade moroten har vildmoroten en tunn, träig pålrot som är ätlig.</t>
   </si>
 </sst>
 </file>
@@ -2406,11 +2409,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R127"/>
+  <dimension ref="A1:S127"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C108" sqref="C108"/>
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2419,12 +2422,12 @@
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="34.140625" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" customWidth="1"/>
-    <col min="15" max="15" width="26.85546875" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" customWidth="1"/>
+    <col min="17" max="17" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="2" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="2" customFormat="1" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2435,7 +2438,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>3</v>
@@ -2455,40 +2458,43 @@
       <c r="J1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>158</v>
+      <c r="K1" s="2" t="s">
+        <v>346</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>157</v>
+        <v>395</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>246</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>316</v>
+        <v>156</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>336</v>
+        <v>230</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -2496,19 +2502,19 @@
       <c r="J2">
         <v>1</v>
       </c>
-      <c r="N2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B3" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C3" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -2519,43 +2525,43 @@
       <c r="J3">
         <v>1</v>
       </c>
-      <c r="N3">
-        <v>2</v>
-      </c>
       <c r="P3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" t="s">
         <v>134</v>
       </c>
-      <c r="C4" t="s">
-        <v>135</v>
-      </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" t="s">
         <v>129</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>130</v>
       </c>
-      <c r="C5" t="s">
-        <v>131</v>
-      </c>
       <c r="D5">
         <v>2</v>
       </c>
@@ -2565,19 +2571,19 @@
       <c r="J5">
         <v>1</v>
       </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -2585,22 +2591,22 @@
       <c r="J6">
         <v>1</v>
       </c>
-      <c r="N6">
-        <v>2</v>
-      </c>
       <c r="P6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -2608,116 +2614,116 @@
       <c r="J7">
         <v>1</v>
       </c>
-      <c r="N7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B8" t="s">
+        <v>203</v>
+      </c>
+      <c r="C8" t="s">
+        <v>204</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>218</v>
+      </c>
+      <c r="B9" t="s">
+        <v>219</v>
+      </c>
+      <c r="C9" t="s">
+        <v>220</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>184</v>
+      </c>
+      <c r="B11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11" t="s">
+        <v>183</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>207</v>
+      </c>
+      <c r="B12" t="s">
         <v>208</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C12" t="s">
         <v>206</v>
       </c>
-      <c r="C8" t="s">
-        <v>207</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="P8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>222</v>
-      </c>
-      <c r="B9" t="s">
-        <v>223</v>
-      </c>
-      <c r="C9" t="s">
-        <v>224</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B10" t="s">
-        <v>127</v>
-      </c>
-      <c r="C10" t="s">
-        <v>126</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>187</v>
-      </c>
-      <c r="B11" t="s">
-        <v>185</v>
-      </c>
-      <c r="C11" t="s">
-        <v>186</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>210</v>
-      </c>
-      <c r="B12" t="s">
-        <v>211</v>
-      </c>
-      <c r="C12" t="s">
-        <v>209</v>
-      </c>
       <c r="D12">
         <v>2</v>
       </c>
       <c r="J12">
         <v>1</v>
       </c>
-      <c r="N12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B13" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C13" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -2725,22 +2731,22 @@
       <c r="J13">
         <v>1</v>
       </c>
-      <c r="L13">
-        <v>1</v>
-      </c>
       <c r="N13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B14" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C14" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -2748,19 +2754,19 @@
       <c r="J14">
         <v>1</v>
       </c>
-      <c r="P14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C15" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -2768,11 +2774,11 @@
       <c r="J15">
         <v>1</v>
       </c>
-      <c r="N15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -2788,337 +2794,337 @@
       <c r="J16">
         <v>1</v>
       </c>
-      <c r="L16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>143</v>
+      </c>
+      <c r="B17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" t="s">
         <v>144</v>
       </c>
-      <c r="B17" t="s">
-        <v>143</v>
-      </c>
-      <c r="C17" t="s">
-        <v>145</v>
-      </c>
       <c r="D17">
         <v>2</v>
       </c>
       <c r="J17">
         <v>1</v>
       </c>
-      <c r="N17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>232</v>
+      </c>
+      <c r="B18" t="s">
+        <v>233</v>
+      </c>
+      <c r="C18" t="s">
+        <v>234</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="P18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>163</v>
+      </c>
+      <c r="B19" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19" t="s">
+        <v>162</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>211</v>
+      </c>
+      <c r="B20" t="s">
+        <v>209</v>
+      </c>
+      <c r="C20" t="s">
+        <v>210</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>236</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B21" t="s">
+        <v>235</v>
+      </c>
+      <c r="C21" t="s">
+        <v>239</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B22" t="s">
+        <v>131</v>
+      </c>
+      <c r="C22" t="s">
+        <v>151</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>223</v>
+      </c>
+      <c r="B23" t="s">
+        <v>221</v>
+      </c>
+      <c r="C23" t="s">
+        <v>222</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>186</v>
+      </c>
+      <c r="B24" t="s">
+        <v>185</v>
+      </c>
+      <c r="C24" t="s">
+        <v>187</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>194</v>
+      </c>
+      <c r="B25" t="s">
+        <v>195</v>
+      </c>
+      <c r="C25" t="s">
+        <v>196</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="R25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>215</v>
+      </c>
+      <c r="B26" t="s">
+        <v>213</v>
+      </c>
+      <c r="C26" t="s">
+        <v>214</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>237</v>
       </c>
-      <c r="C18" t="s">
+      <c r="B27" t="s">
         <v>238</v>
       </c>
-      <c r="D18">
-        <v>2</v>
-      </c>
-      <c r="J18">
-        <v>1</v>
-      </c>
-      <c r="N18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C27" t="s">
+        <v>242</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B28" t="s">
+        <v>137</v>
+      </c>
+      <c r="C28" t="s">
+        <v>138</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>216</v>
+      </c>
+      <c r="B29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C29" t="s">
+        <v>393</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="P29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>164</v>
+      </c>
+      <c r="B30" t="s">
+        <v>166</v>
+      </c>
+      <c r="C30" t="s">
         <v>165</v>
       </c>
-      <c r="B19" t="s">
-        <v>163</v>
-      </c>
-      <c r="C19" t="s">
-        <v>164</v>
-      </c>
-      <c r="D19">
-        <v>2</v>
-      </c>
-      <c r="J19">
-        <v>1</v>
-      </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-      <c r="N19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>214</v>
-      </c>
-      <c r="B20" t="s">
-        <v>212</v>
-      </c>
-      <c r="C20" t="s">
-        <v>213</v>
-      </c>
-      <c r="D20">
-        <v>2</v>
-      </c>
-      <c r="J20">
-        <v>1</v>
-      </c>
-      <c r="N20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>240</v>
-      </c>
-      <c r="B21" t="s">
-        <v>239</v>
-      </c>
-      <c r="C21" t="s">
-        <v>243</v>
-      </c>
-      <c r="D21">
-        <v>2</v>
-      </c>
-      <c r="J21">
-        <v>1</v>
-      </c>
-      <c r="L21">
-        <v>1</v>
-      </c>
-      <c r="N21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="B22" t="s">
-        <v>132</v>
-      </c>
-      <c r="C22" t="s">
-        <v>152</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="J22">
-        <v>1</v>
-      </c>
-      <c r="N22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>227</v>
-      </c>
-      <c r="B23" t="s">
-        <v>225</v>
-      </c>
-      <c r="C23" t="s">
-        <v>226</v>
-      </c>
-      <c r="D23">
-        <v>2</v>
-      </c>
-      <c r="G23">
-        <v>2</v>
-      </c>
-      <c r="H23">
-        <v>2</v>
-      </c>
-      <c r="J23">
-        <v>1</v>
-      </c>
-      <c r="N23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>189</v>
-      </c>
-      <c r="B24" t="s">
-        <v>188</v>
-      </c>
-      <c r="C24" t="s">
-        <v>190</v>
-      </c>
-      <c r="D24">
-        <v>2</v>
-      </c>
-      <c r="J24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>197</v>
-      </c>
-      <c r="B25" t="s">
-        <v>198</v>
-      </c>
-      <c r="C25" t="s">
-        <v>199</v>
-      </c>
-      <c r="D25">
-        <v>2</v>
-      </c>
-      <c r="J25">
-        <v>1</v>
-      </c>
-      <c r="P25">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>218</v>
-      </c>
-      <c r="B26" t="s">
-        <v>216</v>
-      </c>
-      <c r="C26" t="s">
-        <v>217</v>
-      </c>
-      <c r="D26">
-        <v>2</v>
-      </c>
-      <c r="J26">
-        <v>1</v>
-      </c>
-      <c r="L26">
-        <v>1</v>
-      </c>
-      <c r="N26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>241</v>
-      </c>
-      <c r="B27" t="s">
-        <v>242</v>
-      </c>
-      <c r="C27" t="s">
-        <v>246</v>
-      </c>
-      <c r="D27">
-        <v>2</v>
-      </c>
-      <c r="G27">
-        <v>2</v>
-      </c>
-      <c r="J27">
-        <v>1</v>
-      </c>
-      <c r="L27">
-        <v>1</v>
-      </c>
-      <c r="N27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B28" t="s">
-        <v>138</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="P30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>140</v>
+      </c>
+      <c r="B31" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" t="s">
         <v>139</v>
       </c>
-      <c r="D28">
-        <v>2</v>
-      </c>
-      <c r="J28">
-        <v>1</v>
-      </c>
-      <c r="N28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>220</v>
-      </c>
-      <c r="B29" t="s">
-        <v>221</v>
-      </c>
-      <c r="C29" t="s">
-        <v>219</v>
-      </c>
-      <c r="D29">
-        <v>2</v>
-      </c>
-      <c r="J29">
-        <v>1</v>
-      </c>
-      <c r="N29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>166</v>
-      </c>
-      <c r="B30" t="s">
-        <v>168</v>
-      </c>
-      <c r="C30" t="s">
-        <v>167</v>
-      </c>
-      <c r="D30">
-        <v>2</v>
-      </c>
-      <c r="J30">
-        <v>1</v>
-      </c>
-      <c r="N30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>141</v>
-      </c>
-      <c r="B31" t="s">
-        <v>142</v>
-      </c>
-      <c r="C31" t="s">
-        <v>140</v>
-      </c>
       <c r="D31">
         <v>2</v>
       </c>
       <c r="J31">
         <v>1</v>
       </c>
-      <c r="N31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B32" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C32" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -3129,13 +3135,13 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B33" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C33" t="s">
-        <v>176</v>
+        <v>397</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -3143,22 +3149,22 @@
       <c r="J33">
         <v>2</v>
       </c>
-      <c r="N33">
-        <v>2</v>
-      </c>
       <c r="P33">
+        <v>2</v>
+      </c>
+      <c r="R33">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B34" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C34" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="D34">
         <v>2</v>
@@ -3169,40 +3175,40 @@
       <c r="J34">
         <v>2</v>
       </c>
-      <c r="N34">
+      <c r="P34">
         <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>148</v>
+      </c>
+      <c r="B35" t="s">
+        <v>147</v>
+      </c>
+      <c r="C35" t="s">
         <v>149</v>
       </c>
-      <c r="B35" t="s">
-        <v>148</v>
-      </c>
-      <c r="C35" t="s">
-        <v>150</v>
-      </c>
       <c r="D35">
         <v>2</v>
       </c>
       <c r="J35">
         <v>2</v>
       </c>
-      <c r="N35">
+      <c r="P35">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>170</v>
+      </c>
+      <c r="B36" t="s">
+        <v>169</v>
+      </c>
+      <c r="C36" t="s">
         <v>172</v>
       </c>
-      <c r="B36" t="s">
-        <v>171</v>
-      </c>
-      <c r="C36" t="s">
-        <v>174</v>
-      </c>
       <c r="D36">
         <v>2</v>
       </c>
@@ -3212,10 +3218,10 @@
       <c r="J36">
         <v>2</v>
       </c>
-      <c r="L36">
+      <c r="N36">
         <v>3</v>
       </c>
-      <c r="N36">
+      <c r="P36">
         <v>2</v>
       </c>
     </row>
@@ -3238,35 +3244,35 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B38" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C38" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D38">
         <v>2</v>
       </c>
-      <c r="K38">
+      <c r="M38">
         <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B39" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C39" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
-      <c r="N39">
+      <c r="K39">
         <v>1</v>
       </c>
       <c r="P39">
@@ -3281,7 +3287,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C40" t="s">
         <v>53</v>
@@ -3289,19 +3295,19 @@
       <c r="D40">
         <v>2</v>
       </c>
-      <c r="K40">
+      <c r="M40">
         <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B41" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C41" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D41">
         <v>2</v>
@@ -3318,7 +3324,7 @@
         <v>60</v>
       </c>
       <c r="C42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D42">
         <v>2</v>
@@ -3335,13 +3341,13 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B43" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C43" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D43">
         <v>2</v>
@@ -3358,7 +3364,7 @@
         <v>12</v>
       </c>
       <c r="C44" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D44">
         <v>1</v>
@@ -3375,13 +3381,13 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B45" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C45" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D45">
         <v>1</v>
@@ -3415,19 +3421,19 @@
       <c r="H46">
         <v>1</v>
       </c>
-      <c r="L46">
+      <c r="N46">
         <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B47" t="s">
+        <v>158</v>
+      </c>
+      <c r="C47" t="s">
         <v>160</v>
-      </c>
-      <c r="C47" t="s">
-        <v>162</v>
       </c>
       <c r="D47">
         <v>1</v>
@@ -3441,13 +3447,13 @@
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B48" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="C48" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D48">
         <v>2</v>
@@ -3455,19 +3461,19 @@
       <c r="E48">
         <v>1</v>
       </c>
-      <c r="P48">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B49" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C49" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D49">
         <v>2</v>
@@ -3481,19 +3487,19 @@
       <c r="H49">
         <v>2</v>
       </c>
-      <c r="L49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B50" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C50" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="D50">
         <v>2</v>
@@ -3505,7 +3511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -3530,19 +3536,19 @@
       <c r="I51">
         <v>1</v>
       </c>
-      <c r="L51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B52" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C52" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D52">
         <v>1</v>
@@ -3551,15 +3557,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B53" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C53" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D53">
         <v>2</v>
@@ -3570,19 +3576,19 @@
       <c r="G53">
         <v>1</v>
       </c>
-      <c r="P53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>100</v>
+      </c>
+      <c r="B54" t="s">
         <v>101</v>
       </c>
-      <c r="B54" t="s">
-        <v>102</v>
-      </c>
       <c r="C54" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D54">
         <v>2</v>
@@ -3597,15 +3603,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B55" t="s">
         <v>124</v>
       </c>
-      <c r="B55" t="s">
-        <v>125</v>
-      </c>
       <c r="C55" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D55">
         <v>2</v>
@@ -3613,22 +3619,22 @@
       <c r="G55">
         <v>1</v>
       </c>
-      <c r="K55">
+      <c r="M55">
         <v>4</v>
       </c>
-      <c r="N55">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B56" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C56" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D56">
         <v>1</v>
@@ -3639,11 +3645,11 @@
       <c r="H56">
         <v>1</v>
       </c>
-      <c r="P56">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>80</v>
       </c>
@@ -3651,7 +3657,7 @@
         <v>79</v>
       </c>
       <c r="C57" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D57">
         <v>1</v>
@@ -3662,22 +3668,22 @@
       <c r="G57">
         <v>2</v>
       </c>
-      <c r="K57">
-        <v>2</v>
-      </c>
-      <c r="P57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M57">
+        <v>2</v>
+      </c>
+      <c r="R57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B58" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -3686,15 +3692,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>366</v>
+        <v>394</v>
       </c>
       <c r="B59" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C59" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -3702,19 +3708,22 @@
       <c r="G59">
         <v>2</v>
       </c>
-      <c r="P59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L59">
+        <v>1</v>
+      </c>
+      <c r="R59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>98</v>
+      </c>
+      <c r="B60" t="s">
         <v>99</v>
       </c>
-      <c r="B60" t="s">
-        <v>100</v>
-      </c>
       <c r="C60" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D60">
         <v>2</v>
@@ -3729,15 +3738,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B61" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C61" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D61">
         <v>2</v>
@@ -3745,14 +3754,14 @@
       <c r="H61">
         <v>3</v>
       </c>
-      <c r="O61" t="s">
-        <v>235</v>
-      </c>
-      <c r="Q61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q61" t="s">
+        <v>231</v>
+      </c>
+      <c r="S61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>24</v>
       </c>
@@ -3760,7 +3769,7 @@
         <v>25</v>
       </c>
       <c r="C62" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="D62">
         <v>2</v>
@@ -3768,11 +3777,11 @@
       <c r="E62">
         <v>2</v>
       </c>
-      <c r="P62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>59</v>
       </c>
@@ -3792,15 +3801,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B64" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C64" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D64">
         <v>2</v>
@@ -3808,11 +3817,11 @@
       <c r="E64">
         <v>2</v>
       </c>
-      <c r="M64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>71</v>
       </c>
@@ -3820,7 +3829,7 @@
         <v>72</v>
       </c>
       <c r="C65" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D65">
         <v>2</v>
@@ -3832,15 +3841,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B66" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C66" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -3849,7 +3858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>62</v>
       </c>
@@ -3878,7 +3887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>8</v>
       </c>
@@ -3900,22 +3909,22 @@
       <c r="G68">
         <v>1</v>
       </c>
-      <c r="K68">
-        <v>2</v>
-      </c>
-      <c r="P68">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M68">
+        <v>2</v>
+      </c>
+      <c r="R68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="B69" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="C69" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="D69">
         <v>1</v>
@@ -3923,19 +3932,19 @@
       <c r="E69">
         <v>1</v>
       </c>
-      <c r="P69">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B70" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C70" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D70">
         <v>2</v>
@@ -3946,11 +3955,11 @@
       <c r="G70">
         <v>2</v>
       </c>
-      <c r="P70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>44</v>
       </c>
@@ -3963,11 +3972,11 @@
       <c r="D71">
         <v>1</v>
       </c>
-      <c r="K71">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>51</v>
       </c>
@@ -3975,7 +3984,7 @@
         <v>50</v>
       </c>
       <c r="C72" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D72">
         <v>3</v>
@@ -3986,20 +3995,20 @@
       <c r="G72">
         <v>1</v>
       </c>
-      <c r="L72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B73" t="s">
+        <v>270</v>
+      </c>
+      <c r="C73" t="s">
         <v>274</v>
       </c>
-      <c r="C73" t="s">
-        <v>278</v>
-      </c>
       <c r="D73">
         <v>2</v>
       </c>
@@ -4009,19 +4018,19 @@
       <c r="H73">
         <v>2</v>
       </c>
-      <c r="N73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B74" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C74" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -4032,19 +4041,19 @@
       <c r="F74">
         <v>2</v>
       </c>
-      <c r="P74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B75" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C75" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D75">
         <v>2</v>
@@ -4056,15 +4065,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B76" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C76" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D76">
         <v>2</v>
@@ -4073,15 +4082,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B77" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C77" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D77">
         <v>1</v>
@@ -4089,19 +4098,19 @@
       <c r="H77">
         <v>3</v>
       </c>
-      <c r="K77">
+      <c r="M77">
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="B78" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C78" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -4112,11 +4121,11 @@
       <c r="G78">
         <v>1</v>
       </c>
-      <c r="P78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>22</v>
       </c>
@@ -4124,7 +4133,7 @@
         <v>23</v>
       </c>
       <c r="C79" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D79">
         <v>1</v>
@@ -4132,19 +4141,19 @@
       <c r="E79">
         <v>2</v>
       </c>
-      <c r="P79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B80" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C80" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D80">
         <v>2</v>
@@ -4164,36 +4173,36 @@
       <c r="I80">
         <v>1</v>
       </c>
-      <c r="O80" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q80" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B81" t="s">
+        <v>91</v>
+      </c>
+      <c r="C81" t="s">
         <v>93</v>
       </c>
-      <c r="B81" t="s">
-        <v>92</v>
-      </c>
-      <c r="C81" t="s">
-        <v>94</v>
-      </c>
       <c r="D81">
         <v>2</v>
       </c>
-      <c r="K81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B82" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C82" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D82">
         <v>1</v>
@@ -4202,15 +4211,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B83" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C83" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -4224,11 +4233,11 @@
       <c r="G83">
         <v>1</v>
       </c>
-      <c r="P83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>42</v>
       </c>
@@ -4241,19 +4250,19 @@
       <c r="D84">
         <v>3</v>
       </c>
-      <c r="K84">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B85" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C85" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D85">
         <v>2</v>
@@ -4262,7 +4271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>66</v>
       </c>
@@ -4270,27 +4279,27 @@
         <v>65</v>
       </c>
       <c r="C86" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D86">
         <v>2</v>
       </c>
-      <c r="K86">
-        <v>2</v>
-      </c>
-      <c r="L86">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M86">
+        <v>2</v>
+      </c>
+      <c r="N86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B87" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C87" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D87">
         <v>1</v>
@@ -4301,19 +4310,19 @@
       <c r="H87">
         <v>3</v>
       </c>
-      <c r="K87">
+      <c r="M87">
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B88" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C88" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="D88">
         <v>2</v>
@@ -4322,15 +4331,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B89" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C89" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D89">
         <v>2</v>
@@ -4339,15 +4348,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B90" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C90" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D90">
         <v>1</v>
@@ -4362,7 +4371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>16</v>
       </c>
@@ -4385,7 +4394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>19</v>
       </c>
@@ -4402,7 +4411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>70</v>
       </c>
@@ -4410,7 +4419,7 @@
         <v>69</v>
       </c>
       <c r="C93" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D93">
         <v>2</v>
@@ -4428,15 +4437,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>117</v>
+      </c>
+      <c r="B94" t="s">
         <v>118</v>
       </c>
-      <c r="B94" t="s">
-        <v>119</v>
-      </c>
       <c r="C94" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D94">
         <v>1</v>
@@ -4451,15 +4460,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="B95" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="C95" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="D95">
         <v>1</v>
@@ -4467,20 +4476,23 @@
       <c r="G95">
         <v>2</v>
       </c>
-      <c r="P95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L95">
+        <v>1</v>
+      </c>
+      <c r="R95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B96" t="s">
+        <v>305</v>
+      </c>
+      <c r="C96" t="s">
         <v>309</v>
       </c>
-      <c r="C96" t="s">
-        <v>313</v>
-      </c>
       <c r="D96">
         <v>2</v>
       </c>
@@ -4497,15 +4509,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B97" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C97" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="D97">
         <v>1</v>
@@ -4517,7 +4529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>75</v>
       </c>
@@ -4542,36 +4554,36 @@
       <c r="H98">
         <v>1</v>
       </c>
-      <c r="L98">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B99" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C99" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D99">
         <v>2</v>
       </c>
-      <c r="K99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="B100" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="C100" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="D100">
         <v>1</v>
@@ -4579,19 +4591,19 @@
       <c r="E100">
         <v>1</v>
       </c>
-      <c r="P100">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B101" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C101" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D101">
         <v>1</v>
@@ -4603,7 +4615,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>46</v>
       </c>
@@ -4611,7 +4623,7 @@
         <v>45</v>
       </c>
       <c r="C102" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D102">
         <v>2</v>
@@ -4622,19 +4634,19 @@
       <c r="G102">
         <v>1</v>
       </c>
-      <c r="K102">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M102">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B103" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C103" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D103">
         <v>2</v>
@@ -4645,11 +4657,11 @@
       <c r="H103">
         <v>3</v>
       </c>
-      <c r="O103" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q103" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>27</v>
       </c>
@@ -4657,7 +4669,7 @@
         <v>26</v>
       </c>
       <c r="C104" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D104">
         <v>1</v>
@@ -4672,15 +4684,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B105" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="C105" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D105">
         <v>1</v>
@@ -4691,19 +4703,19 @@
       <c r="F105">
         <v>1</v>
       </c>
-      <c r="P105">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B106" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C106" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D106">
         <v>2</v>
@@ -4711,19 +4723,19 @@
       <c r="G106">
         <v>2</v>
       </c>
-      <c r="L106">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="B107" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C107" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="D107">
         <v>1</v>
@@ -4737,19 +4749,19 @@
       <c r="G107">
         <v>2</v>
       </c>
-      <c r="P107">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="B108" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C108" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="D108">
         <v>1</v>
@@ -4757,19 +4769,22 @@
       <c r="G108">
         <v>1</v>
       </c>
-      <c r="P108">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L108">
+        <v>1</v>
+      </c>
+      <c r="R108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B109" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C109" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D109">
         <v>1</v>
@@ -4777,19 +4792,19 @@
       <c r="G109">
         <v>2</v>
       </c>
-      <c r="K109">
+      <c r="M109">
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B110" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C110" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D110">
         <v>1</v>
@@ -4800,19 +4815,19 @@
       <c r="F110">
         <v>2</v>
       </c>
-      <c r="P110">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="B111" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C111" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="D111">
         <v>1</v>
@@ -4823,31 +4838,31 @@
       <c r="F111">
         <v>1</v>
       </c>
-      <c r="P111">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="R111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>154</v>
+      </c>
+      <c r="B112" t="s">
+        <v>153</v>
+      </c>
+      <c r="C112" t="s">
         <v>155</v>
       </c>
-      <c r="B112" t="s">
-        <v>154</v>
-      </c>
-      <c r="C112" t="s">
-        <v>156</v>
-      </c>
       <c r="D112">
         <v>2</v>
       </c>
-      <c r="K112">
-        <v>1</v>
-      </c>
-      <c r="N112">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M112">
+        <v>1</v>
+      </c>
+      <c r="P112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>40</v>
       </c>
@@ -4855,7 +4870,7 @@
         <v>39</v>
       </c>
       <c r="C113" t="s">
-        <v>82</v>
+        <v>398</v>
       </c>
       <c r="D113">
         <v>2</v>
@@ -4864,7 +4879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>67</v>
       </c>
@@ -4872,24 +4887,24 @@
         <v>68</v>
       </c>
       <c r="C114" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D114">
         <v>1</v>
       </c>
-      <c r="K114">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B115" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C115" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D115">
         <v>2</v>
@@ -4910,15 +4925,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B116" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C116" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D116">
         <v>1</v>
@@ -4933,7 +4948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>13</v>
       </c>
@@ -4956,7 +4971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>29</v>
       </c>
@@ -4979,15 +4994,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B119" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C119" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D119">
         <v>1</v>
@@ -5002,7 +5017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>32</v>
       </c>
@@ -5025,15 +5040,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B121" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C121" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D121">
         <v>2</v>
@@ -5045,35 +5060,35 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B122" t="s">
+        <v>227</v>
+      </c>
+      <c r="C122" t="s">
+        <v>229</v>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+      <c r="H122">
+        <v>2</v>
+      </c>
+      <c r="Q122" t="s">
         <v>231</v>
       </c>
-      <c r="C122" t="s">
-        <v>233</v>
-      </c>
-      <c r="D122">
-        <v>1</v>
-      </c>
-      <c r="H122">
-        <v>2</v>
-      </c>
-      <c r="O122" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B123" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C123" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D123">
         <v>2</v>
@@ -5088,88 +5103,88 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="B124" t="s">
+        <v>380</v>
+      </c>
+      <c r="C124" t="s">
+        <v>385</v>
+      </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
+      <c r="J124">
+        <v>1</v>
+      </c>
+      <c r="R124">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>386</v>
+      </c>
+      <c r="B125" t="s">
+        <v>381</v>
+      </c>
+      <c r="C125" t="s">
+        <v>387</v>
+      </c>
+      <c r="D125">
+        <v>1</v>
+      </c>
+      <c r="J125">
+        <v>1</v>
+      </c>
+      <c r="R125">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>390</v>
+      </c>
+      <c r="B126" t="s">
+        <v>382</v>
+      </c>
+      <c r="C126" t="s">
+        <v>391</v>
+      </c>
+      <c r="D126">
+        <v>2</v>
+      </c>
+      <c r="J126">
+        <v>1</v>
+      </c>
+      <c r="R126">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>389</v>
       </c>
-      <c r="B124" t="s">
-        <v>385</v>
-      </c>
-      <c r="C124" t="s">
-        <v>390</v>
-      </c>
-      <c r="D124">
-        <v>1</v>
-      </c>
-      <c r="J124">
-        <v>1</v>
-      </c>
-      <c r="P124">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>391</v>
-      </c>
-      <c r="B125" t="s">
-        <v>386</v>
-      </c>
-      <c r="C125" t="s">
-        <v>392</v>
-      </c>
-      <c r="D125">
-        <v>1</v>
-      </c>
-      <c r="J125">
-        <v>1</v>
-      </c>
-      <c r="P125">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>395</v>
-      </c>
-      <c r="B126" t="s">
-        <v>387</v>
-      </c>
-      <c r="C126" t="s">
-        <v>396</v>
-      </c>
-      <c r="D126">
-        <v>2</v>
-      </c>
-      <c r="J126">
-        <v>1</v>
-      </c>
-      <c r="P126">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>394</v>
-      </c>
       <c r="B127" t="s">
+        <v>383</v>
+      </c>
+      <c r="C127" t="s">
         <v>388</v>
       </c>
-      <c r="C127" t="s">
-        <v>393</v>
-      </c>
       <c r="D127">
         <v>1</v>
       </c>
       <c r="J127">
         <v>1</v>
       </c>
-      <c r="P127">
+      <c r="R127">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R126">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S126">
     <sortCondition ref="J2:J126"/>
     <sortCondition ref="B2:B126"/>
   </sortState>

</xml_diff>

<commit_message>
Plants added, fungus fix
* Added more plants
		* Fixed fungus not showing
		[Android Build: 75Mb] Added more plants [total 138, pictures: 204]
</commit_message>
<xml_diff>
--- a/Assets/Data/Plants.xlsx
+++ b/Assets/Data/Plants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Unity Projects\GitHub\Edible Plants\Assets\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE0AFB8-C9E4-4812-A50D-EA23B08E3AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3169BDB7-45B8-4D2E-A7E1-233D0CB8C196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="443">
   <si>
     <t>Latin Name</t>
   </si>
@@ -1536,6 +1536,138 @@
   </si>
   <si>
     <t>Vildmorot (Daucus carota) är en art i familjen flockblommiga växter. I likhet med alla övriga arter i morotssläktet är växten tvåårig. Den förädlade moroten (D. carota sativa) klassas som en underart. Den förekommer i Eurasien och Nordafrika. Människan har spridit den till Amerika, där den blivit ett svårt ogräs. Till skillnad från den förädlade moroten har vildmoroten en tunn, träig pålrot som är ätlig.</t>
+  </si>
+  <si>
+    <t>Lomme</t>
+  </si>
+  <si>
+    <t>Capsella bursa-pastoris</t>
+  </si>
+  <si>
+    <t>Penningört (Thlaspi arvense) är ett mycket vanligt åker- och trädgårdsogräs, lite mindre vanligt i Skandinaviens nordliga delar. Penningörten har fått sitt svenska namn efter sina stora, runda skidor, vilka liknats vid mynt. Dess vetenskapliga artepitet, arvense, har betydelsen "växande på åkrar". Bladen vissnar snabbt och kan göra plantan nästan bladlös. Bladen kan ätas som sallad men smakar ganska starkt. Växten producerar stora mängder frön och hela förskidorna kan användas på samma sätt som krasse.</t>
+  </si>
+  <si>
+    <t>Thlaspi arvense</t>
+  </si>
+  <si>
+    <t>Lomme (även kallat lommegräs, lommeört) (Capsella bursa-pastoris) är en växtart i familjen korsblommiga växter. Lomme är ett av de vanligaste ogräsen i hela Norden. På våren kan man skörda lommen innan blomstjälkarna kommer upp. Smaken påminner om krasse och kan användas på samma sätt. Smaken kan vara lite pikant så man äter helst inga stora mängder. Historiskt har man pressat olja ur fröna på samma sätt som andra korsblommiga växter såsom raps. Lommen kan ibland angripas av svamp och bör då undvikas.</t>
+  </si>
+  <si>
+    <t>Penningört</t>
+  </si>
+  <si>
+    <t>Bitterkrassing (Lepidium latifolium) är en växtart i familjen korsblommiga växter. Den växer vid havsstränder och ibland vid avfallsplatser. Bladen, skotten och frukterna är ätliga. De smakar skarpt och har historiskt använts som pepparrot. Bitterheten och pepparsmaken kan mildras genom kokning och sedan urlakning. Sedan kan växten användas som spenat.</t>
+  </si>
+  <si>
+    <t>Lepidium latifolium</t>
+  </si>
+  <si>
+    <t>Bitterkrassing</t>
+  </si>
+  <si>
+    <t>Gatkrassing</t>
+  </si>
+  <si>
+    <t>Lepidium ruderale</t>
+  </si>
+  <si>
+    <t>Gatkrassing (Lepidium ruderale.) ibland kallad gatkrasse, är en växt i familjen korsblommiga växter. Det är en vild släkting till smörgåskrassen och kan användas på samma sätt. Örten luktar likt senap och kan av vissaq upplevas som obehaglig.</t>
+  </si>
+  <si>
+    <t>Marviol (Cakile maritima) är en ört med blekt rödlila blommor. Marviol är en strandväxt som är vanlig längs havskusterna i södra Sverige, men som kan förekomma ända upp till Västerbotten. Den växer både på sandstränder och stenstränder. Stjälkarna är blågröna och köttiga. Skidorna har en smak av ättika. Små blad kan ätas som sallad och har en senapslikanande smak och innehåller en del C-vitamin. Blad och stjälkar kan kokas till soppa.</t>
+  </si>
+  <si>
+    <t>Marviol</t>
+  </si>
+  <si>
+    <t>Cakile maritima</t>
+  </si>
+  <si>
+    <t>Strandkål</t>
+  </si>
+  <si>
+    <t>Blekinge, Gotland</t>
+  </si>
+  <si>
+    <t>Sverige</t>
+  </si>
+  <si>
+    <t>Crambe maritima</t>
+  </si>
+  <si>
+    <t>Strandkålen är en flerårig, kal ört, upp till 80 cm hög med ett både djupgående och utbrett rotsystem. Bladen är stora, krusiga och blågröna, de nedre har långa skaft. Strandkålen äår vanligare på västkusten än på östkusten. Den odlas framför allt i England som en delikatess. Unga blad och skott kan användas som spenat medan äldre delar kan kokas och användas som kål. Smaken är nötliknande. Strandkålen är fridlyst i Blekinge och i Gotlands län.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Åkerrättika (Raphanus raphanistrum) hittas ofta namnet säger på åkrar. Den anträffas i nästan alla sädesodlande trakter av Finland, Sverige och Norge, utom i de mest nordligaste delarna. Unga skott hos örten kan ätas som sallad. Fröna kan ätas men smakar lite bittert. </t>
+  </si>
+  <si>
+    <t>Åkerrättika</t>
+  </si>
+  <si>
+    <t>Raphanus raphanistrum</t>
+  </si>
+  <si>
+    <t>Brassica rapa ssp. campestris</t>
+  </si>
+  <si>
+    <t>Åkerkål</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Åkerkål (Brassica rapa ssp. campestris) är en ettårig meterhög ört med gula blommor som blommar från juni till juli. Förekommer i hela Sverige och anses vara ett ogräs på många platser. Den hybridiserar ofta med rovor och rybs.  </t>
+  </si>
+  <si>
+    <t>Sumpfräne (Rorippa palustris) är en växtart i familjen korsblommiga växter. Det är ettårig eller tvåårig ört med ljusgula blommor och parflikiga blad som trivs på fuktig mark. Fröna kan användas som senap. Det sägs att växten används för att väcka liv i skendöda personer.</t>
+  </si>
+  <si>
+    <t>Rorippa palustris</t>
+  </si>
+  <si>
+    <t>Sumpfräne</t>
+  </si>
+  <si>
+    <t>Brassica nigra</t>
+  </si>
+  <si>
+    <t>Svartsenap</t>
+  </si>
+  <si>
+    <t>Vitsenap (Sinapis alba) är en art i familjen korsblommiga växter och förekommer naturligt från östra Medelhavsområdet till sydvästra Asien och Indien. Arten odlas som krydd- och medicinalväxt, men kan också användas till att bekämpa nematoder i odlingar. Det är en ettårig ört och har trots sitt namn gula blommor. Ur vitsenapens frö utvinns olja som används för att göra senap, men på senare tid har vitsenapen också fått konkurrens från sareptasenapen (Brassica juncea), även kallad brun senap, eftersom denna är enklare att skörda med maskin. Starkare varianter av senap, till exempel skånsk senap, använder istället en viss mängd frö från svartsenap (S. nigra) för att få en starkare smak.</t>
+  </si>
+  <si>
+    <t>Vitsenap</t>
+  </si>
+  <si>
+    <t>Sinapis alba</t>
+  </si>
+  <si>
+    <t>Sinapis arvensis</t>
+  </si>
+  <si>
+    <t>Åkersenap</t>
+  </si>
+  <si>
+    <t>Åkersenap (Sinapis arvensis) art i familjen korsblommiga växter och hör till de vanligast och rikast förekommande ettåriga ogräsen i åkrar och andra odlingar i Sverige. Den förekommer naturligt i Europa och Nordafrika. Fröna kan användas som senap men har en svag senapssmak.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Svartsenap (Brassica nigra) är en ettårig växt som tillhör kålsläktet och familjen korsblommiga växter. Den tillhör alltså inte, som till exempel åkersenapen och vitsenapen, släktet senaper (Sinapis), utan bara samma familj. Svartsenap är sällsynt och sällan naturaliserad men odlades förr. Svartsenapens frö används framför allt till framställning av starkare senapssorter, exempelvis skånsk senap och fransk dijonsenap. De vanliga sorterna av senap görs istället med frö från vitsenapen, men båda dessa arter har på senare tid fått konkurrens ifrån den indiska brunsenapen (Brassica juncea) eftersom dess frö är enklare att skörda maskinellt. </t>
+  </si>
+  <si>
+    <t>Berberis</t>
+  </si>
+  <si>
+    <t>Berberis vulgaris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Berberis (Berberis vulgaris), ibland kallad surtorn, är en växtart i familjen berberisväxter som förekommer naturligt i Iran, Turkiet och Kaukasus. Till Europa infördes växten som läkeväxt och finns numera naturaliserad. Berberis har förvildats i stora delar av Sverige. Busken blommar med gula blommor och bildar sedan klarröda klasar av avlånga bär. Bären har en frisk och syrlig smak och används till sylt, saft och gele. Bären har tidigare används istället för citron. Under en stor del av 1900-talet ansågs växten fredlöst och skulle utrotas under den så kallade berberislagen, då den är invasiv och bärare av svartrosten , en parasit som angriper sädesslag. </t>
+  </si>
+  <si>
+    <t>Näckrosor</t>
+  </si>
+  <si>
+    <t>Nymphaeaceae</t>
+  </si>
+  <si>
+    <t>Näckrosväxter (Nymphaeaceae) är en växtfamilj där plantorna växer i stillastående eller långsamt strömmande sötvatten. Roten är giftig men har ändå använts historiskt. Den har malts till mjöl och slammats flera gånger för att få bort gifterna. Undvik.</t>
   </si>
 </sst>
 </file>
@@ -2047,13 +2179,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="16" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2409,11 +2542,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S127"/>
+  <dimension ref="A1:S141"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C113" sqref="C113"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C142" sqref="C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2424,6 +2557,7 @@
     <col min="4" max="4" width="10.42578125" customWidth="1"/>
     <col min="13" max="13" width="15.42578125" customWidth="1"/>
     <col min="14" max="14" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" customWidth="1"/>
     <col min="17" max="17" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3817,8 +3951,8 @@
       <c r="E64">
         <v>2</v>
       </c>
-      <c r="O64">
-        <v>1</v>
+      <c r="O64" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
@@ -5181,6 +5315,301 @@
       </c>
       <c r="R127">
         <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>400</v>
+      </c>
+      <c r="B128" t="s">
+        <v>399</v>
+      </c>
+      <c r="C128" t="s">
+        <v>403</v>
+      </c>
+      <c r="D128">
+        <v>1</v>
+      </c>
+      <c r="F128">
+        <v>1</v>
+      </c>
+      <c r="G128">
+        <v>1</v>
+      </c>
+      <c r="I128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>402</v>
+      </c>
+      <c r="B129" t="s">
+        <v>404</v>
+      </c>
+      <c r="C129" t="s">
+        <v>401</v>
+      </c>
+      <c r="D129">
+        <v>1</v>
+      </c>
+      <c r="F129">
+        <v>1</v>
+      </c>
+      <c r="G129">
+        <v>1</v>
+      </c>
+      <c r="I129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>406</v>
+      </c>
+      <c r="B130" t="s">
+        <v>407</v>
+      </c>
+      <c r="C130" t="s">
+        <v>405</v>
+      </c>
+      <c r="D130">
+        <v>1</v>
+      </c>
+      <c r="F130">
+        <v>1</v>
+      </c>
+      <c r="G130">
+        <v>1</v>
+      </c>
+      <c r="I130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>409</v>
+      </c>
+      <c r="B131" t="s">
+        <v>408</v>
+      </c>
+      <c r="C131" t="s">
+        <v>410</v>
+      </c>
+      <c r="D131">
+        <v>1</v>
+      </c>
+      <c r="F131">
+        <v>1</v>
+      </c>
+      <c r="G131">
+        <v>1</v>
+      </c>
+      <c r="H131">
+        <v>1</v>
+      </c>
+      <c r="I131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>413</v>
+      </c>
+      <c r="B132" t="s">
+        <v>412</v>
+      </c>
+      <c r="C132" t="s">
+        <v>411</v>
+      </c>
+      <c r="D132">
+        <v>2</v>
+      </c>
+      <c r="F132">
+        <v>2</v>
+      </c>
+      <c r="G132">
+        <v>1</v>
+      </c>
+      <c r="H132">
+        <v>1</v>
+      </c>
+      <c r="I132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>417</v>
+      </c>
+      <c r="B133" t="s">
+        <v>414</v>
+      </c>
+      <c r="C133" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="D133">
+        <v>2</v>
+      </c>
+      <c r="F133">
+        <v>1</v>
+      </c>
+      <c r="G133">
+        <v>1</v>
+      </c>
+      <c r="O133" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>421</v>
+      </c>
+      <c r="B134" t="s">
+        <v>420</v>
+      </c>
+      <c r="C134" t="s">
+        <v>419</v>
+      </c>
+      <c r="D134">
+        <v>2</v>
+      </c>
+      <c r="F134">
+        <v>1</v>
+      </c>
+      <c r="G134">
+        <v>1</v>
+      </c>
+      <c r="I134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>422</v>
+      </c>
+      <c r="B135" t="s">
+        <v>423</v>
+      </c>
+      <c r="C135" t="s">
+        <v>424</v>
+      </c>
+      <c r="D135">
+        <v>2</v>
+      </c>
+      <c r="F135">
+        <v>1</v>
+      </c>
+      <c r="G135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>426</v>
+      </c>
+      <c r="B136" t="s">
+        <v>427</v>
+      </c>
+      <c r="C136" t="s">
+        <v>425</v>
+      </c>
+      <c r="D136">
+        <v>2</v>
+      </c>
+      <c r="I136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>428</v>
+      </c>
+      <c r="B137" t="s">
+        <v>429</v>
+      </c>
+      <c r="C137" t="s">
+        <v>436</v>
+      </c>
+      <c r="D137">
+        <v>2</v>
+      </c>
+      <c r="I137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>432</v>
+      </c>
+      <c r="B138" t="s">
+        <v>431</v>
+      </c>
+      <c r="C138" t="s">
+        <v>430</v>
+      </c>
+      <c r="D138">
+        <v>2</v>
+      </c>
+      <c r="I138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>433</v>
+      </c>
+      <c r="B139" t="s">
+        <v>434</v>
+      </c>
+      <c r="C139" t="s">
+        <v>435</v>
+      </c>
+      <c r="D139">
+        <v>2</v>
+      </c>
+      <c r="I139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>438</v>
+      </c>
+      <c r="B140" t="s">
+        <v>437</v>
+      </c>
+      <c r="C140" t="s">
+        <v>439</v>
+      </c>
+      <c r="D140">
+        <v>2</v>
+      </c>
+      <c r="J140">
+        <v>1</v>
+      </c>
+      <c r="N140">
+        <v>1</v>
+      </c>
+      <c r="P140">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>441</v>
+      </c>
+      <c r="B141" t="s">
+        <v>440</v>
+      </c>
+      <c r="C141" t="s">
+        <v>442</v>
+      </c>
+      <c r="D141">
+        <v>2</v>
+      </c>
+      <c r="M141">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -5193,8 +5622,11 @@
     <hyperlink ref="C94" r:id="rId2" location="Förklara_sammanhanget" tooltip="Wikipedia:Inledning och sammanhang" display="https://sv.wikipedia.org/wiki/Wikipedia:Inledning_och_sammanhang - Förklara_sammanhanget" xr:uid="{73307867-6B81-4F73-B236-36C8832E5A5D}"/>
     <hyperlink ref="C95" r:id="rId3" tooltip="Luftförorening" display="https://sv.wikipedia.org/wiki/Luftf%C3%B6rorening" xr:uid="{A972A4F6-1CD6-4FB0-814B-16AE61A337C7}"/>
     <hyperlink ref="C127" r:id="rId4" tooltip="Buske" display="https://sv.wikipedia.org/wiki/Buske" xr:uid="{D2FA3C8A-A4DD-47BF-A488-3E13AA0B3D01}"/>
+    <hyperlink ref="C129" r:id="rId5" tooltip="Ogräs" display="https://sv.wikipedia.org/wiki/Ogr%C3%A4s" xr:uid="{60632165-9332-412F-8615-1B69BD3C2F64}"/>
+    <hyperlink ref="C131" r:id="rId6" display="https://sv.wikipedia.org/wiki/Korsblommiga_v%C3%A4xter" xr:uid="{06A93DC0-DA1D-47C6-ADD7-87CF227E25E1}"/>
+    <hyperlink ref="C141" r:id="rId7" tooltip="Familj (biologi)" display="https://sv.wikipedia.org/wiki/Familj_(biologi)" xr:uid="{09B4B8BD-676A-466F-92F7-EFDF3730B0F5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>